<commit_message>
sum impressive shit right here
</commit_message>
<xml_diff>
--- a/Results/Forecast Evaluation Results.xlsx
+++ b/Results/Forecast Evaluation Results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="27360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="1440" yWindow="460" windowWidth="27360" windowHeight="15820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAE" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="117">
   <si>
     <t>SSM</t>
   </si>
@@ -73,6 +73,312 @@
   </si>
   <si>
     <t>SSM2</t>
+  </si>
+  <si>
+    <t>SSM 1</t>
+  </si>
+  <si>
+    <t>0.0168455494381603</t>
+  </si>
+  <si>
+    <t>0.0215290466027630</t>
+  </si>
+  <si>
+    <t>0.0270618087686418</t>
+  </si>
+  <si>
+    <t>0.0326400801328880</t>
+  </si>
+  <si>
+    <t>0.0405282456325865</t>
+  </si>
+  <si>
+    <t>0.0403796895473277</t>
+  </si>
+  <si>
+    <t>0.0431961935520005</t>
+  </si>
+  <si>
+    <t>0.0455930279650950</t>
+  </si>
+  <si>
+    <t>0.0477074066588990</t>
+  </si>
+  <si>
+    <t>0.0491635242081847</t>
+  </si>
+  <si>
+    <t>0.0503666631328860</t>
+  </si>
+  <si>
+    <t>0.0518588499518567</t>
+  </si>
+  <si>
+    <t>0.0531266673736455</t>
+  </si>
+  <si>
+    <t>0.0541946050160739</t>
+  </si>
+  <si>
+    <t>0.0537646101458288</t>
+  </si>
+  <si>
+    <t>0.0551431246965534</t>
+  </si>
+  <si>
+    <t>0.0304959083453174</t>
+  </si>
+  <si>
+    <t>0.0332000474737596</t>
+  </si>
+  <si>
+    <t>0.0335713546472300</t>
+  </si>
+  <si>
+    <t>0.0363109872586046</t>
+  </si>
+  <si>
+    <t>0.0401622545169493</t>
+  </si>
+  <si>
+    <t>0.0453289086281628</t>
+  </si>
+  <si>
+    <t>0.0523828713086356</t>
+  </si>
+  <si>
+    <t>0.0615564571812309</t>
+  </si>
+  <si>
+    <t>0.0722089984407520</t>
+  </si>
+  <si>
+    <t>0.0848456003718344</t>
+  </si>
+  <si>
+    <t>0.0994754942952828</t>
+  </si>
+  <si>
+    <t>0.113618334615791</t>
+  </si>
+  <si>
+    <t>0.150890531248610</t>
+  </si>
+  <si>
+    <t>0.173934033345095</t>
+  </si>
+  <si>
+    <t>0.215470547808813</t>
+  </si>
+  <si>
+    <t>0.247977748976655</t>
+  </si>
+  <si>
+    <t>0.298252789193216</t>
+  </si>
+  <si>
+    <t>0.341365418751215</t>
+  </si>
+  <si>
+    <t>0.402445438778567</t>
+  </si>
+  <si>
+    <t>0.459674222309368</t>
+  </si>
+  <si>
+    <t>0.529179031164694</t>
+  </si>
+  <si>
+    <t>0.601616102460833</t>
+  </si>
+  <si>
+    <t>0.689664445961613</t>
+  </si>
+  <si>
+    <t>0.740830448126348</t>
+  </si>
+  <si>
+    <t>0.120237643114441</t>
+  </si>
+  <si>
+    <t>0.133773107729736</t>
+  </si>
+  <si>
+    <t>0.143361934069381</t>
+  </si>
+  <si>
+    <t>0.155033873921686</t>
+  </si>
+  <si>
+    <t>0.168848873915720</t>
+  </si>
+  <si>
+    <t>0.180996105806038</t>
+  </si>
+  <si>
+    <t>0.195527106230029</t>
+  </si>
+  <si>
+    <t>0.209552979841174</t>
+  </si>
+  <si>
+    <t>0.214362328510550</t>
+  </si>
+  <si>
+    <t>0.228786556843855</t>
+  </si>
+  <si>
+    <t>0.241468195157781</t>
+  </si>
+  <si>
+    <t>0.214204006064968</t>
+  </si>
+  <si>
+    <t>SSM 2</t>
+  </si>
+  <si>
+    <t>0.00908036297342884</t>
+  </si>
+  <si>
+    <t>0.0128418183700519</t>
+  </si>
+  <si>
+    <t>0.0159322296335964</t>
+  </si>
+  <si>
+    <t>0.0181861965762496</t>
+  </si>
+  <si>
+    <t>0.0193113771758482</t>
+  </si>
+  <si>
+    <t>0.0215808184502354</t>
+  </si>
+  <si>
+    <t>0.0212986652293820</t>
+  </si>
+  <si>
+    <t>0.0226764573780497</t>
+  </si>
+  <si>
+    <t>0.0245370884074586</t>
+  </si>
+  <si>
+    <t>0.0266584261373996</t>
+  </si>
+  <si>
+    <t>0.0296083092910703</t>
+  </si>
+  <si>
+    <t>0.0327284060702530</t>
+  </si>
+  <si>
+    <t>0.0364548344452102</t>
+  </si>
+  <si>
+    <t>0.0413761929443983</t>
+  </si>
+  <si>
+    <t>0.0468381255598651</t>
+  </si>
+  <si>
+    <t>0.0495062104453424</t>
+  </si>
+  <si>
+    <t>0.0220847636912200</t>
+  </si>
+  <si>
+    <t>0.0376845559117715</t>
+  </si>
+  <si>
+    <t>0.0554176666256622</t>
+  </si>
+  <si>
+    <t>0.0656600696543094</t>
+  </si>
+  <si>
+    <t>0.0805612720530228</t>
+  </si>
+  <si>
+    <t>0.0904181297587195</t>
+  </si>
+  <si>
+    <t>0.105102366440970</t>
+  </si>
+  <si>
+    <t>0.116025623443817</t>
+  </si>
+  <si>
+    <t>0.131630579126671</t>
+  </si>
+  <si>
+    <t>0.141424668034083</t>
+  </si>
+  <si>
+    <t>0.157895175683388</t>
+  </si>
+  <si>
+    <t>0.173650426855346</t>
+  </si>
+  <si>
+    <t>0.182226387992815</t>
+  </si>
+  <si>
+    <t>0.199007654329133</t>
+  </si>
+  <si>
+    <t>0.218357735295837</t>
+  </si>
+  <si>
+    <t>0.201538468536669</t>
+  </si>
+  <si>
+    <t>0.0208504688628743</t>
+  </si>
+  <si>
+    <t>0.0374491638864840</t>
+  </si>
+  <si>
+    <t>0.0528001115982745</t>
+  </si>
+  <si>
+    <t>0.0636838276286855</t>
+  </si>
+  <si>
+    <t>0.0777275186317444</t>
+  </si>
+  <si>
+    <t>0.0873624561820285</t>
+  </si>
+  <si>
+    <t>0.0943748456347091</t>
+  </si>
+  <si>
+    <t>0.102904832870164</t>
+  </si>
+  <si>
+    <t>0.114329997031986</t>
+  </si>
+  <si>
+    <t>0.122307919294604</t>
+  </si>
+  <si>
+    <t>0.133952994057859</t>
+  </si>
+  <si>
+    <t>0.144790900145211</t>
+  </si>
+  <si>
+    <t>0.146368447957193</t>
+  </si>
+  <si>
+    <t>0.154485550054511</t>
+  </si>
+  <si>
+    <t>0.158540323752474</t>
+  </si>
+  <si>
+    <t>0.146093746588162</t>
   </si>
 </sst>
 </file>
@@ -132,7 +438,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -140,8 +446,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -152,26 +468,35 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -447,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z62"/>
+  <dimension ref="A1:Z66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L57" sqref="L57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,453 +787,621 @@
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>8</v>
       </c>
-      <c r="G2">
+      <c r="G3">
         <v>12</v>
       </c>
-      <c r="H2">
+      <c r="H3">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <f>B35/B35</f>
         <v>1</v>
       </c>
-      <c r="D3">
-        <f t="shared" ref="D3:H3" si="0">C35/C35</f>
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="2">
-        <f>B40/B35</f>
-        <v>1.0942028985507246</v>
-      </c>
-      <c r="D4" s="2">
-        <f t="shared" ref="D4:H4" si="1">C40/C35</f>
-        <v>1.0246913580246915</v>
-      </c>
-      <c r="E4" s="2">
-        <f t="shared" si="1"/>
-        <v>0.98514851485148525</v>
-      </c>
-      <c r="F4" s="2">
-        <f t="shared" si="1"/>
-        <v>0.95862068965517233</v>
-      </c>
-      <c r="G4" s="2">
-        <f t="shared" si="1"/>
-        <v>0.9840000000000001</v>
-      </c>
-      <c r="H4" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0159453302961274</v>
+      <c r="D4">
+        <f>C35/C35</f>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f>D35/D35</f>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <f>E35/E35</f>
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <f>F35/F35</f>
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <f>G35/G35</f>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="2">
-        <f>B45/B35</f>
-        <v>1.4057971014492754</v>
+        <f>B40/B35</f>
+        <v>1.0942028985507246</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" ref="D5:H5" si="2">C45/C35</f>
-        <v>1.2222222222222223</v>
+        <f>C40/C35</f>
+        <v>1.0246913580246915</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0594059405940595</v>
+        <f>D40/D35</f>
+        <v>0.98514851485148525</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="2"/>
-        <v>0.87931034482758608</v>
+        <f>E40/E35</f>
+        <v>0.95862068965517233</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="2"/>
-        <v>0.84266666666666679</v>
+        <f>F40/F35</f>
+        <v>0.9840000000000001</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="2"/>
-        <v>0.82687927107061499</v>
+        <f>G40/G35</f>
+        <v>1.0159453302961274</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <f>B45/B35</f>
+        <v>1.4057971014492754</v>
+      </c>
+      <c r="D6" s="2">
+        <f>C45/C35</f>
+        <v>1.2222222222222223</v>
+      </c>
+      <c r="E6" s="2">
+        <f>D45/D35</f>
+        <v>1.0594059405940595</v>
+      </c>
+      <c r="F6" s="2">
+        <f>E45/E35</f>
+        <v>0.87931034482758608</v>
+      </c>
+      <c r="G6" s="2">
+        <f>F45/F35</f>
+        <v>0.84266666666666679</v>
+      </c>
+      <c r="H6" s="2">
+        <f>G45/G35</f>
+        <v>0.82687927107061499</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C7" s="2">
         <f>B50/B35</f>
         <v>0.63768115942028991</v>
       </c>
-      <c r="D6" s="2">
-        <f t="shared" ref="D6:H6" si="3">C50/C35</f>
+      <c r="D7" s="2">
+        <f>C50/C35</f>
         <v>0.69753086419753085</v>
       </c>
-      <c r="E6" s="2">
-        <f t="shared" si="3"/>
+      <c r="E7" s="2">
+        <f>D50/D35</f>
         <v>0.76732673267326734</v>
       </c>
-      <c r="F6" s="2">
-        <f t="shared" si="3"/>
+      <c r="F7" s="2">
+        <f>E50/E35</f>
         <v>0.52068965517241383</v>
       </c>
-      <c r="G6" s="2">
-        <f t="shared" si="3"/>
+      <c r="G7" s="2">
+        <f>F50/F35</f>
         <v>0.38133333333333336</v>
       </c>
-      <c r="H6" s="2">
-        <f t="shared" si="3"/>
+      <c r="H7" s="2">
+        <f>G50/G35</f>
         <v>0.33940774487471526</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2">
+        <f>B55/B35</f>
+        <v>0.79192631102819566</v>
+      </c>
+      <c r="D8" s="2">
+        <f>C55/C35</f>
+        <v>0.96816371548238278</v>
+      </c>
+      <c r="E8" s="2">
+        <f>D55/D35</f>
+        <v>1.3578365183468268</v>
+      </c>
+      <c r="F8" s="2">
+        <f>E55/E35</f>
+        <v>1.2623532402044171</v>
+      </c>
+      <c r="G8" s="2">
+        <f>F55/F35</f>
+        <v>1.1703426660463014</v>
+      </c>
+      <c r="H8" s="2">
+        <f>G55/G35</f>
+        <v>1.1452690165955284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2">
+        <f>B60/B35</f>
+        <v>0.65799731691513341</v>
+      </c>
+      <c r="D9" s="2">
+        <f>C60/C35</f>
+        <v>0.79270483765752475</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D60/D35</f>
+        <v>0.90030676120047515</v>
+      </c>
+      <c r="F9" s="2">
+        <f>E60/E35</f>
+        <v>0.78194680613964473</v>
+      </c>
+      <c r="G9" s="2">
+        <f>F60/F35</f>
+        <v>0.87275749520674673</v>
+      </c>
+      <c r="H9" s="2">
+        <f>G60/G35</f>
+        <v>1.127704110372264</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
         <v>2</v>
       </c>
-      <c r="E8">
+      <c r="E11">
         <v>4</v>
       </c>
-      <c r="F8">
+      <c r="F11">
         <v>8</v>
       </c>
-      <c r="G8">
+      <c r="G11">
         <v>12</v>
       </c>
-      <c r="H8">
+      <c r="H11">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C9">
+      <c r="C12">
         <f>B41/B41</f>
         <v>1</v>
       </c>
-      <c r="D9">
-        <f t="shared" ref="D9:G9" si="4">C41/C41</f>
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="H9">
+      <c r="D12">
+        <f>C41/C41</f>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f>D41/D41</f>
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <f>E41/E41</f>
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <f>F41/F41</f>
+        <v>1</v>
+      </c>
+      <c r="H12">
         <f>G41/G41</f>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C13" s="2">
         <f>B41/B36</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D10" s="2">
-        <f t="shared" ref="D10:H10" si="5">C41/C36</f>
+      <c r="D13" s="2">
+        <f>C41/C36</f>
         <v>0.93103448275862077</v>
       </c>
-      <c r="E10" s="2">
-        <f t="shared" si="5"/>
+      <c r="E13" s="2">
+        <f>D41/D36</f>
         <v>1.1142857142857141</v>
       </c>
-      <c r="F10" s="2">
-        <f t="shared" si="5"/>
+      <c r="F13" s="2">
+        <f>E41/E36</f>
         <v>0.89583333333333337</v>
       </c>
-      <c r="G10" s="2">
-        <f t="shared" si="5"/>
+      <c r="G13" s="2">
+        <f>F41/F36</f>
         <v>0.7</v>
       </c>
-      <c r="H10" s="2">
-        <f t="shared" si="5"/>
+      <c r="H13" s="2">
+        <f>G41/G36</f>
         <v>0.44871794871794873</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C14" s="2">
         <f>B46/B36</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="D11" s="2">
-        <f t="shared" ref="D11:H11" si="6">C46/C36</f>
+      <c r="D14" s="2">
+        <f>C46/C36</f>
         <v>0.93103448275862077</v>
       </c>
-      <c r="E11" s="2">
-        <f t="shared" si="6"/>
+      <c r="E14" s="2">
+        <f>D46/D36</f>
         <v>1.1142857142857141</v>
       </c>
-      <c r="F11" s="2">
-        <f t="shared" si="6"/>
+      <c r="F14" s="2">
+        <f>E46/E36</f>
         <v>0.875</v>
       </c>
-      <c r="G11" s="2">
-        <f t="shared" si="6"/>
+      <c r="G14" s="2">
+        <f>F46/F36</f>
         <v>0.68571428571428561</v>
       </c>
-      <c r="H11" s="2">
-        <f t="shared" si="6"/>
+      <c r="H14" s="2">
+        <f>G46/G36</f>
         <v>0.4358974358974359</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C15" s="2">
         <f>B51/B36</f>
         <v>1.8888888888888888</v>
       </c>
-      <c r="D12" s="2">
-        <f t="shared" ref="D12:H12" si="7">C51/C36</f>
+      <c r="D15" s="2">
+        <f>C51/C36</f>
         <v>3</v>
       </c>
-      <c r="E12" s="2">
-        <f t="shared" si="7"/>
+      <c r="E15" s="2">
+        <f>D51/D36</f>
         <v>2.5714285714285712</v>
       </c>
-      <c r="F12" s="2">
-        <f t="shared" si="7"/>
+      <c r="F15" s="2">
+        <f>E51/E36</f>
         <v>2.2083333333333335</v>
       </c>
-      <c r="G12" s="2">
-        <f t="shared" si="7"/>
+      <c r="G15" s="2">
+        <f>F51/F36</f>
         <v>1.5857142857142859</v>
       </c>
-      <c r="H12" s="2">
-        <f t="shared" si="7"/>
+      <c r="H15" s="2">
+        <f>G51/G36</f>
         <v>1.8076923076923077</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>4</v>
-      </c>
-      <c r="F14">
-        <v>8</v>
-      </c>
-      <c r="G14">
-        <v>12</v>
-      </c>
-      <c r="H14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <f>B47/B47</f>
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <f t="shared" ref="D15:H15" si="8">C47/C47</f>
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="8"/>
-        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="2">
+        <f>B56/B36</f>
+        <v>1.9192823130175556</v>
+      </c>
+      <c r="D16" s="2">
+        <f>C56/C36</f>
+        <v>3.1098555423629137</v>
+      </c>
+      <c r="E16" s="2">
+        <f>D56/D36</f>
+        <v>4.0972192655231714</v>
+      </c>
+      <c r="F16" s="2">
+        <f>E56/E36</f>
+        <v>2.6331337943585833</v>
+      </c>
+      <c r="G16" s="2">
+        <f>F56/F36</f>
+        <v>2.0830446574182</v>
+      </c>
+      <c r="H16" s="2">
+        <f>G56/G36</f>
+        <v>2.1171214629621411</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2">
+        <f>B61/B36</f>
+        <v>8.1795421078592589</v>
+      </c>
+      <c r="D17" s="2">
+        <f>C61/C36</f>
+        <v>12.994674452335001</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D61/D36</f>
+        <v>18.760019901231257</v>
+      </c>
+      <c r="F17" s="2">
+        <f>E61/E36</f>
+        <v>24.172004884128544</v>
+      </c>
+      <c r="G17" s="2">
+        <f>F61/F36</f>
+        <v>24.807203836478003</v>
+      </c>
+      <c r="H17" s="2">
+        <f>G61/G36</f>
+        <v>25.838265197008848</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="F19">
         <v>8</v>
       </c>
-      <c r="C16" s="2">
+      <c r="G19">
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <f>B47/B47</f>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>C47/C47</f>
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <f>D47/D47</f>
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <f>E47/E47</f>
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <f>F47/F47</f>
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <f>G47/G47</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="2">
         <f>B42/B37</f>
         <v>0.27407407407407408</v>
       </c>
-      <c r="D16" s="2">
-        <f t="shared" ref="D16:H16" si="9">C42/C37</f>
+      <c r="D21" s="2">
+        <f>C42/C37</f>
         <v>0.38815789473684209</v>
       </c>
-      <c r="E16" s="2">
-        <f t="shared" si="9"/>
+      <c r="E21" s="2">
+        <f>D42/D37</f>
         <v>0.62962962962962976</v>
       </c>
-      <c r="F16" s="2">
-        <f t="shared" si="9"/>
+      <c r="F21" s="2">
+        <f>E42/E37</f>
         <v>0.91219512195121955</v>
       </c>
-      <c r="G16" s="2">
-        <f t="shared" si="9"/>
+      <c r="G21" s="2">
+        <f>F42/F37</f>
         <v>1.0941176470588236</v>
       </c>
-      <c r="H16" s="2">
-        <f t="shared" si="9"/>
+      <c r="H21" s="2">
+        <f>G42/G37</f>
         <v>1.4891304347826086</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C22" s="2">
         <f>B47/B37</f>
         <v>0.25925925925925924</v>
       </c>
-      <c r="D17" s="2">
-        <f t="shared" ref="D17:H17" si="10">C47/C37</f>
+      <c r="D22" s="2">
+        <f>C47/C37</f>
         <v>0.36184210526315785</v>
       </c>
-      <c r="E17" s="2">
-        <f t="shared" si="10"/>
+      <c r="E22" s="2">
+        <f>D47/D37</f>
         <v>0.54320987654320996</v>
       </c>
-      <c r="F17" s="2">
-        <f t="shared" si="10"/>
+      <c r="F22" s="2">
+        <f>E47/E37</f>
         <v>0.76585365853658527</v>
       </c>
-      <c r="G17" s="2">
-        <f t="shared" si="10"/>
+      <c r="G22" s="2">
+        <f>F47/F37</f>
         <v>0.90196078431372551</v>
       </c>
-      <c r="H17" s="2">
-        <f t="shared" si="10"/>
+      <c r="H22" s="2">
+        <f>G47/G37</f>
         <v>1.1847826086956521</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C23" s="2">
         <f>B52/B37</f>
         <v>0.48148148148148145</v>
       </c>
-      <c r="D18" s="2">
-        <f t="shared" ref="D18:H18" si="11">C52/C37</f>
+      <c r="D23" s="2">
+        <f>C52/C37</f>
         <v>0.74342105263157887</v>
       </c>
-      <c r="E18" s="2">
-        <f t="shared" si="11"/>
+      <c r="E23" s="2">
+        <f>D52/D37</f>
         <v>0.97530864197530875</v>
       </c>
-      <c r="F18" s="2">
-        <f t="shared" si="11"/>
+      <c r="F23" s="2">
+        <f>E52/E37</f>
         <v>0.82439024390243887</v>
       </c>
-      <c r="G18" s="2">
-        <f t="shared" si="11"/>
+      <c r="G23" s="2">
+        <f>F52/F37</f>
         <v>0.81176470588235294</v>
       </c>
-      <c r="H18" s="2">
-        <f t="shared" si="11"/>
+      <c r="H23" s="2">
+        <f>G52/G37</f>
         <v>0.92028985507246375</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2">
+        <f>B57/B37</f>
+        <v>0.51581563387925777</v>
+      </c>
+      <c r="D24" s="2">
+        <f>C57/C37</f>
+        <v>0.73633405738570401</v>
+      </c>
+      <c r="E24" s="2">
+        <f>D57/D37</f>
+        <v>1.1938080124980617</v>
+      </c>
+      <c r="F24" s="2">
+        <f>E57/E37</f>
+        <v>0.87511521982990237</v>
+      </c>
+      <c r="G24" s="2">
+        <f>F57/F37</f>
+        <v>0.94340042327306672</v>
+      </c>
+      <c r="H24" s="2">
+        <f>G57/G37</f>
+        <v>1.5038884836762065</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="2">
+        <f>B62/B37</f>
+        <v>1.544479175027726</v>
+      </c>
+      <c r="D25" s="2">
+        <f>C62/C37</f>
+        <v>2.4637607820055263</v>
+      </c>
+      <c r="E25" s="2">
+        <f>D62/D37</f>
+        <v>3.9311004709065127</v>
+      </c>
+      <c r="F25" s="2">
+        <f>E62/E37</f>
+        <v>5.0197479448860483</v>
+      </c>
+      <c r="G25" s="2">
+        <f>F62/F37</f>
+        <v>5.6780745154984711</v>
+      </c>
+      <c r="H25" s="2">
+        <f>G62/G37</f>
+        <v>5.2932516879768841</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1257,23 +1750,23 @@
       <c r="A55" t="s">
         <v>4</v>
       </c>
-      <c r="B55" s="9">
-        <v>6.2415856651729402E-3</v>
-      </c>
-      <c r="C55" s="9">
-        <v>8.2129366995989106E-3</v>
-      </c>
-      <c r="D55" s="9">
-        <v>1.08242454678328E-2</v>
-      </c>
-      <c r="E55" s="9">
-        <v>1.4103862338652601E-2</v>
-      </c>
-      <c r="F55" s="9">
-        <v>1.54833755611152E-2</v>
-      </c>
-      <c r="G55" s="9">
-        <v>1.7069635722301298E-2</v>
+      <c r="B55" s="7">
+        <v>1.09285830921891E-2</v>
+      </c>
+      <c r="C55" s="7">
+        <v>1.5684252190814599E-2</v>
+      </c>
+      <c r="D55" s="7">
+        <v>2.7428297670605901E-2</v>
+      </c>
+      <c r="E55" s="7">
+        <v>3.66082439659281E-2</v>
+      </c>
+      <c r="F55" s="7">
+        <v>4.3887849976736303E-2</v>
+      </c>
+      <c r="G55" s="7">
+        <v>5.0277309828543698E-2</v>
       </c>
       <c r="K55">
         <v>8.0052891059123193E-3</v>
@@ -1328,23 +1821,23 @@
       <c r="A56" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="9">
-        <v>2.3733447801932298E-3</v>
-      </c>
-      <c r="C56" s="9">
-        <v>4.6718933204455797E-3</v>
-      </c>
-      <c r="D56" s="9">
-        <v>7.2079935591526497E-3</v>
-      </c>
-      <c r="E56" s="9">
-        <v>1.16841045329142E-2</v>
-      </c>
-      <c r="F56" s="9">
-        <v>1.4506432461196799E-2</v>
-      </c>
-      <c r="G56" s="9">
-        <v>1.80590775479068E-2</v>
+      <c r="B56" s="7">
+        <v>5.1820622451474001E-3</v>
+      </c>
+      <c r="C56" s="7">
+        <v>9.0185810728524492E-3</v>
+      </c>
+      <c r="D56" s="7">
+        <v>1.43402674293311E-2</v>
+      </c>
+      <c r="E56" s="7">
+        <v>1.2639042212921199E-2</v>
+      </c>
+      <c r="F56" s="7">
+        <v>1.4581312601927399E-2</v>
+      </c>
+      <c r="G56" s="7">
+        <v>1.6513547411104699E-2</v>
       </c>
       <c r="K56">
         <v>7.2332208679299296E-3</v>
@@ -1399,23 +1892,23 @@
       <c r="A57" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="9">
-        <v>3.5187480976608702E-3</v>
-      </c>
-      <c r="C57" s="9">
-        <v>6.00947252872809E-3</v>
-      </c>
-      <c r="D57" s="9">
-        <v>9.9326296671946208E-3</v>
-      </c>
-      <c r="E57" s="9">
-        <v>1.41488131567173E-2</v>
-      </c>
-      <c r="F57" s="9">
-        <v>1.20026313865384E-2</v>
-      </c>
-      <c r="G57" s="9">
-        <v>1.60213959540631E-2</v>
+      <c r="B57" s="7">
+        <v>6.9635110573699798E-3</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1.1192277672262701E-2</v>
+      </c>
+      <c r="D57" s="7">
+        <v>1.9339689802468599E-2</v>
+      </c>
+      <c r="E57" s="7">
+        <v>1.7939862006512999E-2</v>
+      </c>
+      <c r="F57" s="7">
+        <v>2.40567107934632E-2</v>
+      </c>
+      <c r="G57" s="7">
+        <v>4.1507322149463302E-2</v>
       </c>
       <c r="K57">
         <v>9.7655222529229192E-3</v>
@@ -1475,15 +1968,363 @@
       <c r="A60" t="s">
         <v>4</v>
       </c>
+      <c r="B60" s="7">
+        <v>9.0803629734288408E-3</v>
+      </c>
+      <c r="C60" s="7">
+        <v>1.28418183700519E-2</v>
+      </c>
+      <c r="D60" s="7">
+        <v>1.8186196576249598E-2</v>
+      </c>
+      <c r="E60" s="7">
+        <v>2.26764573780497E-2</v>
+      </c>
+      <c r="F60" s="7">
+        <v>3.2728406070252999E-2</v>
+      </c>
+      <c r="G60" s="7">
+        <v>4.9506210445342397E-2</v>
+      </c>
+      <c r="K60">
+        <v>1.09285830921891E-2</v>
+      </c>
+      <c r="L60">
+        <v>1.5684252190814599E-2</v>
+      </c>
+      <c r="M60">
+        <v>2.1988096721545398E-2</v>
+      </c>
+      <c r="N60">
+        <v>2.7428297670605901E-2</v>
+      </c>
+      <c r="O60">
+        <v>3.1995202439044301E-2</v>
+      </c>
+      <c r="P60">
+        <v>3.6643754099371102E-2</v>
+      </c>
+      <c r="Q60">
+        <v>3.43591341060017E-2</v>
+      </c>
+      <c r="R60">
+        <v>3.66082439659281E-2</v>
+      </c>
+      <c r="S60">
+        <v>3.8430630162800898E-2</v>
+      </c>
+      <c r="T60">
+        <v>4.0008182623722702E-2</v>
+      </c>
+      <c r="U60">
+        <v>4.18642725056819E-2</v>
+      </c>
+      <c r="V60">
+        <v>4.3887849976736303E-2</v>
+      </c>
+      <c r="W60">
+        <v>4.5952192989651398E-2</v>
+      </c>
+      <c r="X60">
+        <v>4.7189274525062101E-2</v>
+      </c>
+      <c r="Y60">
+        <v>4.9078754947618403E-2</v>
+      </c>
+      <c r="Z60">
+        <v>5.0277309828543698E-2</v>
+      </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>5</v>
       </c>
+      <c r="B61" s="7">
+        <v>2.2084763691220002E-2</v>
+      </c>
+      <c r="C61" s="7">
+        <v>3.76845559117715E-2</v>
+      </c>
+      <c r="D61" s="7">
+        <v>6.56600696543094E-2</v>
+      </c>
+      <c r="E61" s="7">
+        <v>0.11602562344381701</v>
+      </c>
+      <c r="F61" s="7">
+        <v>0.17365042685534601</v>
+      </c>
+      <c r="G61" s="7">
+        <v>0.20153846853666901</v>
+      </c>
+      <c r="K61">
+        <v>5.1820622451474001E-3</v>
+      </c>
+      <c r="L61">
+        <v>9.0185810728524492E-3</v>
+      </c>
+      <c r="M61">
+        <v>1.20141748672534E-2</v>
+      </c>
+      <c r="N61">
+        <v>1.43402674293311E-2</v>
+      </c>
+      <c r="O61">
+        <v>1.6647852364622E-2</v>
+      </c>
+      <c r="P61">
+        <v>1.6642882098932801E-2</v>
+      </c>
+      <c r="Q61">
+        <v>1.51823357381634E-2</v>
+      </c>
+      <c r="R61">
+        <v>1.2639042212921199E-2</v>
+      </c>
+      <c r="S61">
+        <v>1.33846299779823E-2</v>
+      </c>
+      <c r="T61">
+        <v>1.39569375417057E-2</v>
+      </c>
+      <c r="U61">
+        <v>1.39744874073944E-2</v>
+      </c>
+      <c r="V61">
+        <v>1.4581312601927399E-2</v>
+      </c>
+      <c r="W61">
+        <v>1.4868631598005199E-2</v>
+      </c>
+      <c r="X61">
+        <v>1.53134670208811E-2</v>
+      </c>
+      <c r="Y61">
+        <v>1.52371964281613E-2</v>
+      </c>
+      <c r="Z61">
+        <v>1.6513547411104699E-2</v>
+      </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>6</v>
+      </c>
+      <c r="B62" s="7">
+        <v>2.08504688628743E-2</v>
+      </c>
+      <c r="C62" s="7">
+        <v>3.7449163886483998E-2</v>
+      </c>
+      <c r="D62" s="7">
+        <v>6.3683827628685505E-2</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0.102904832870164</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0.14479090014521101</v>
+      </c>
+      <c r="G62" s="7">
+        <v>0.14609374658816199</v>
+      </c>
+      <c r="K62">
+        <v>6.9635110573699798E-3</v>
+      </c>
+      <c r="L62">
+        <v>1.1192277672262701E-2</v>
+      </c>
+      <c r="M62">
+        <v>1.55584030354018E-2</v>
+      </c>
+      <c r="N62">
+        <v>1.9339689802468599E-2</v>
+      </c>
+      <c r="O62">
+        <v>2.3364639244223901E-2</v>
+      </c>
+      <c r="P62">
+        <v>2.5053652432396802E-2</v>
+      </c>
+      <c r="Q62">
+        <v>2.32392484871452E-2</v>
+      </c>
+      <c r="R62">
+        <v>1.7939862006512999E-2</v>
+      </c>
+      <c r="S62">
+        <v>1.9514495101156801E-2</v>
+      </c>
+      <c r="T62">
+        <v>2.09557883338365E-2</v>
+      </c>
+      <c r="U62">
+        <v>2.2207942644404399E-2</v>
+      </c>
+      <c r="V62">
+        <v>2.40567107934632E-2</v>
+      </c>
+      <c r="W62">
+        <v>2.7719350428003699E-2</v>
+      </c>
+      <c r="X62">
+        <v>3.1765286420225497E-2</v>
+      </c>
+      <c r="Y62">
+        <v>3.6388851509567798E-2</v>
+      </c>
+      <c r="Z62">
+        <v>4.1507322149463302E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="K64" t="s">
+        <v>69</v>
+      </c>
+      <c r="L64" t="s">
+        <v>70</v>
+      </c>
+      <c r="M64" t="s">
+        <v>71</v>
+      </c>
+      <c r="N64" t="s">
+        <v>72</v>
+      </c>
+      <c r="O64" t="s">
+        <v>73</v>
+      </c>
+      <c r="P64" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q64" t="s">
+        <v>75</v>
+      </c>
+      <c r="R64" t="s">
+        <v>76</v>
+      </c>
+      <c r="S64" t="s">
+        <v>77</v>
+      </c>
+      <c r="T64" t="s">
+        <v>78</v>
+      </c>
+      <c r="U64" t="s">
+        <v>79</v>
+      </c>
+      <c r="V64" t="s">
+        <v>80</v>
+      </c>
+      <c r="W64" t="s">
+        <v>81</v>
+      </c>
+      <c r="X64" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="65" spans="11:26" x14ac:dyDescent="0.2">
+      <c r="K65" t="s">
+        <v>85</v>
+      </c>
+      <c r="L65" t="s">
+        <v>86</v>
+      </c>
+      <c r="M65" t="s">
+        <v>87</v>
+      </c>
+      <c r="N65" t="s">
+        <v>88</v>
+      </c>
+      <c r="O65" t="s">
+        <v>89</v>
+      </c>
+      <c r="P65" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q65" t="s">
+        <v>91</v>
+      </c>
+      <c r="R65" t="s">
+        <v>92</v>
+      </c>
+      <c r="S65" t="s">
+        <v>93</v>
+      </c>
+      <c r="T65" t="s">
+        <v>94</v>
+      </c>
+      <c r="U65" t="s">
+        <v>95</v>
+      </c>
+      <c r="V65" t="s">
+        <v>96</v>
+      </c>
+      <c r="W65" t="s">
+        <v>97</v>
+      </c>
+      <c r="X65" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="11:26" x14ac:dyDescent="0.2">
+      <c r="K66" t="s">
+        <v>101</v>
+      </c>
+      <c r="L66" t="s">
+        <v>102</v>
+      </c>
+      <c r="M66" t="s">
+        <v>103</v>
+      </c>
+      <c r="N66" t="s">
+        <v>104</v>
+      </c>
+      <c r="O66" t="s">
+        <v>105</v>
+      </c>
+      <c r="P66" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q66" t="s">
+        <v>107</v>
+      </c>
+      <c r="R66" t="s">
+        <v>108</v>
+      </c>
+      <c r="S66" t="s">
+        <v>109</v>
+      </c>
+      <c r="T66" t="s">
+        <v>110</v>
+      </c>
+      <c r="U66" t="s">
+        <v>111</v>
+      </c>
+      <c r="V66" t="s">
+        <v>112</v>
+      </c>
+      <c r="W66" t="s">
+        <v>113</v>
+      </c>
+      <c r="X66" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1497,10 +2338,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:Z63"/>
   <sheetViews>
-    <sheetView topLeftCell="I31" workbookViewId="0">
-      <selection activeCell="M56" sqref="M56:AB58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1512,553 +2353,604 @@
       <c r="B1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E3" s="5">
         <v>4</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F3" s="5">
         <v>8</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G3" s="5">
         <v>12</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H3" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>1</v>
-      </c>
-      <c r="H3" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="10">
-        <f>B41/B36</f>
-        <v>1.3666666666666667</v>
-      </c>
-      <c r="D4" s="10">
-        <f t="shared" ref="D4:H4" si="0">C41/C36</f>
-        <v>1.1612903225806452</v>
-      </c>
-      <c r="E4" s="10">
-        <f t="shared" si="0"/>
-        <v>0.96491228070175439</v>
-      </c>
-      <c r="F4" s="10">
-        <f t="shared" si="0"/>
-        <v>0.83170731707317069</v>
-      </c>
-      <c r="G4" s="10">
-        <f t="shared" si="0"/>
-        <v>0.79923518164435947</v>
-      </c>
-      <c r="H4" s="10">
-        <f t="shared" si="0"/>
-        <v>0.77151799687010947</v>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5">
+        <v>1</v>
+      </c>
+      <c r="H4" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="10">
-        <f>B46/B36</f>
+        <v>8</v>
+      </c>
+      <c r="C5" s="8">
+        <f>B41/B36</f>
         <v>1.3666666666666667</v>
       </c>
-      <c r="D5" s="10">
-        <f t="shared" ref="D5:H5" si="1">C46/C36</f>
-        <v>1.1520737327188941</v>
-      </c>
-      <c r="E5" s="10">
-        <f t="shared" si="1"/>
-        <v>0.94736842105263153</v>
-      </c>
-      <c r="F5" s="10">
-        <f t="shared" si="1"/>
-        <v>0.80487804878048785</v>
-      </c>
-      <c r="G5" s="10">
-        <f t="shared" si="1"/>
-        <v>0.76099426386233271</v>
-      </c>
-      <c r="H5" s="10">
-        <f t="shared" si="1"/>
-        <v>0.72300469483568075</v>
+      <c r="D5" s="8">
+        <f>C41/C36</f>
+        <v>1.1612903225806452</v>
+      </c>
+      <c r="E5" s="8">
+        <f>D41/D36</f>
+        <v>0.96491228070175439</v>
+      </c>
+      <c r="F5" s="8">
+        <f>E41/E36</f>
+        <v>0.83170731707317069</v>
+      </c>
+      <c r="G5" s="8">
+        <f>F41/F36</f>
+        <v>0.79923518164435947</v>
+      </c>
+      <c r="H5" s="8">
+        <f>G41/G36</f>
+        <v>0.77151799687010947</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8">
+        <f>B46/B36</f>
+        <v>1.3666666666666667</v>
+      </c>
+      <c r="D6" s="8">
+        <f>C46/C36</f>
+        <v>1.1520737327188941</v>
+      </c>
+      <c r="E6" s="8">
+        <f>D46/D36</f>
+        <v>0.94736842105263153</v>
+      </c>
+      <c r="F6" s="8">
+        <f>E46/E36</f>
+        <v>0.80487804878048785</v>
+      </c>
+      <c r="G6" s="8">
+        <f>F46/F36</f>
+        <v>0.76099426386233271</v>
+      </c>
+      <c r="H6" s="8">
+        <f>G46/G36</f>
+        <v>0.72300469483568075</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C7" s="8">
         <f>B51/B36</f>
         <v>0.78333333333333333</v>
       </c>
-      <c r="D6" s="10">
-        <f t="shared" ref="D6:H6" si="2">C51/C36</f>
+      <c r="D7" s="8">
+        <f>C51/C36</f>
         <v>0.87096774193548387</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="2"/>
+      <c r="E7" s="8">
+        <f>D51/D36</f>
         <v>0.94035087719298249</v>
       </c>
-      <c r="F6" s="10">
-        <f t="shared" si="2"/>
+      <c r="F7" s="8">
+        <f>E51/E36</f>
         <v>0.51707317073170733</v>
       </c>
-      <c r="G6" s="10">
-        <f t="shared" si="2"/>
+      <c r="G7" s="8">
+        <f>F51/F36</f>
         <v>0.39388145315487572</v>
       </c>
-      <c r="H6" s="10">
-        <f t="shared" si="2"/>
+      <c r="H7" s="8">
+        <f>G51/G36</f>
         <v>0.31611893583724571</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="10">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8">
         <f>B56/B36</f>
-        <v>0.51893450877435165</v>
-      </c>
-      <c r="D7" s="10">
-        <f t="shared" ref="D7:H7" si="3">C56/C36</f>
-        <v>0.62236440753321198</v>
-      </c>
-      <c r="E7" s="10">
-        <f t="shared" si="3"/>
-        <v>0.70090707564054033</v>
-      </c>
-      <c r="F7" s="10">
-        <f t="shared" si="3"/>
-        <v>0.66526943427239515</v>
-      </c>
-      <c r="G7" s="10">
-        <f t="shared" si="3"/>
-        <v>0.58040569942290632</v>
-      </c>
-      <c r="H7" s="10">
-        <f t="shared" si="3"/>
-        <v>0.49811418627618315</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="11">
+        <v>0.93586385767557234</v>
+      </c>
+      <c r="D8" s="8">
+        <f>C56/C36</f>
+        <v>0.99212196326096769</v>
+      </c>
+      <c r="E8" s="8">
+        <f>D56/D36</f>
+        <v>1.1452659695750176</v>
+      </c>
+      <c r="F8" s="8">
+        <f>D56/E36</f>
+        <v>0.79609951543629265</v>
+      </c>
+      <c r="G8" s="8">
+        <f>E56/F36</f>
+        <v>0.87175961692342252</v>
+      </c>
+      <c r="H8" s="8">
+        <f>G56/G36</f>
+        <v>0.86295969791163385</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="2">
         <f>B61/B36</f>
-        <v>0</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5">
-        <v>1</v>
-      </c>
-      <c r="D10" s="5">
+        <v>0.76873279423509444</v>
+      </c>
+      <c r="D9" s="2">
+        <f>C61/C36</f>
+        <v>0.87808305741398618</v>
+      </c>
+      <c r="E9" s="2">
+        <f>D61/D36</f>
+        <v>0.98640732372795781</v>
+      </c>
+      <c r="F9" s="2">
+        <f>E61/E36</f>
+        <v>0.88563383557572184</v>
+      </c>
+      <c r="G9" s="2">
+        <f>F61/F36</f>
+        <v>1.176987709010151</v>
+      </c>
+      <c r="H9" s="2">
+        <f>G61/G36</f>
+        <v>1.7780647044724727</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5">
         <v>2</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E11" s="5">
         <v>4</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F11" s="5">
         <v>8</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G11" s="5">
         <v>12</v>
       </c>
-      <c r="H10" s="5">
+      <c r="H11" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="5">
-        <v>1</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1</v>
-      </c>
-      <c r="H11" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="10">
-        <f>B42/B37</f>
-        <v>0.72727272727272718</v>
-      </c>
-      <c r="D12" s="10">
-        <f>C42/C37</f>
-        <v>1.027027027027027</v>
-      </c>
-      <c r="E12" s="10">
-        <f>D42/D37</f>
-        <v>0.94827586206896552</v>
-      </c>
-      <c r="F12" s="10">
-        <f>E42/E37</f>
-        <v>0.54</v>
-      </c>
-      <c r="G12" s="10">
-        <f>F42/F37</f>
-        <v>0.3202247191011236</v>
-      </c>
-      <c r="H12" s="10">
-        <f>G42/G37</f>
-        <v>0.17355371900826447</v>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="10">
-        <f>B47/B37</f>
-        <v>0.69696969696969702</v>
-      </c>
-      <c r="D13" s="10">
-        <f>C47/C37</f>
-        <v>0.97297297297297292</v>
-      </c>
-      <c r="E13" s="10">
-        <f>D47/D37</f>
-        <v>0.86206896551724144</v>
-      </c>
-      <c r="F13" s="10">
-        <f>E47/E37</f>
-        <v>0.52</v>
-      </c>
-      <c r="G13" s="10">
-        <f>F47/F37</f>
-        <v>0.33146067415730335</v>
-      </c>
-      <c r="H13" s="10">
-        <f>G47/G37</f>
+        <v>8</v>
+      </c>
+      <c r="C13" s="8">
+        <f>B42/B37</f>
+        <v>0.72727272727272718</v>
+      </c>
+      <c r="D13" s="8">
+        <f>C42/C37</f>
+        <v>1.027027027027027</v>
+      </c>
+      <c r="E13" s="8">
+        <f>D42/D37</f>
+        <v>0.94827586206896552</v>
+      </c>
+      <c r="F13" s="8">
+        <f>E42/E37</f>
+        <v>0.54</v>
+      </c>
+      <c r="G13" s="8">
+        <f>F42/F37</f>
+        <v>0.3202247191011236</v>
+      </c>
+      <c r="H13" s="8">
+        <f>G42/G37</f>
         <v>0.17355371900826447</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="8">
+        <f>B47/B37</f>
+        <v>0.69696969696969702</v>
+      </c>
+      <c r="D14" s="8">
+        <f>C47/C37</f>
+        <v>0.97297297297297292</v>
+      </c>
+      <c r="E14" s="8">
+        <f>D47/D37</f>
+        <v>0.86206896551724144</v>
+      </c>
+      <c r="F14" s="8">
+        <f>E47/E37</f>
+        <v>0.52</v>
+      </c>
+      <c r="G14" s="8">
+        <f>F47/F37</f>
+        <v>0.33146067415730335</v>
+      </c>
+      <c r="H14" s="8">
+        <f>G47/G37</f>
+        <v>0.17355371900826447</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C15" s="8">
         <f>B52/B37</f>
         <v>4.5757575757575761</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D15" s="8">
         <f>C52/C37</f>
         <v>6.6216216216216219</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E15" s="8">
         <f>D52/D37</f>
         <v>3.0689655172413794</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F15" s="8">
         <f>E52/E37</f>
         <v>1.68</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G15" s="8">
         <f>F52/F37</f>
         <v>0.9044943820224719</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H15" s="8">
         <f>G52/G37</f>
         <v>0.79752066115702491</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="4"/>
-      <c r="B15" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="10">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="8">
         <f>B57/B37</f>
-        <v>0.94961739445320614</v>
-      </c>
-      <c r="D15" s="10">
-        <f t="shared" ref="D15:H15" si="4">C57/C37</f>
-        <v>1.7286266135249242</v>
-      </c>
-      <c r="E15" s="10">
-        <f t="shared" si="4"/>
-        <v>1.9849667419532071</v>
-      </c>
-      <c r="F15" s="10">
-        <f t="shared" si="4"/>
-        <v>2.0019766955538398</v>
-      </c>
-      <c r="G15" s="10">
-        <f t="shared" si="4"/>
-        <v>1.5333286100402135</v>
-      </c>
-      <c r="H15" s="10">
-        <f t="shared" si="4"/>
-        <v>1.435857119093314</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5">
-        <v>1</v>
-      </c>
-      <c r="D18" s="5">
+        <v>3.2652260698906064</v>
+      </c>
+      <c r="D16" s="8">
+        <f>C57/C37</f>
+        <v>5.1032677568286751</v>
+      </c>
+      <c r="E16" s="8">
+        <f>D57/D37</f>
+        <v>5.2549759255712933</v>
+      </c>
+      <c r="F16" s="8">
+        <f>D57/E37</f>
+        <v>3.0478860368313501</v>
+      </c>
+      <c r="G16" s="8">
+        <f>E57/F37</f>
+        <v>1.3398340388935788</v>
+      </c>
+      <c r="H16" s="8">
+        <f>G57/G37</f>
+        <v>1.3451237614623512</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C17" s="2">
+        <f>B62/B37</f>
+        <v>12.631264848748666</v>
+      </c>
+      <c r="D17" s="2">
+        <f>C62/C37</f>
+        <v>17.027264875454811</v>
+      </c>
+      <c r="E17" s="2">
+        <f>D62/D37</f>
+        <v>19.93284651766724</v>
+      </c>
+      <c r="F17" s="2">
+        <f>E62/E37</f>
+        <v>24.797774897665501</v>
+      </c>
+      <c r="G17" s="2">
+        <f>F62/F37</f>
+        <v>25.824394511762247</v>
+      </c>
+      <c r="H17" s="2">
+        <f>G62/G37</f>
+        <v>30.612828434973061</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E19" s="5">
         <v>4</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F19" s="5">
         <v>8</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G19" s="5">
         <v>12</v>
       </c>
-      <c r="H18" s="5">
+      <c r="H19" s="5">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="5">
-        <v>1</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5">
-        <v>1</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
-      </c>
-      <c r="G19" s="5">
-        <v>1</v>
-      </c>
-      <c r="H19" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="10">
-        <f>B43/B38</f>
-        <v>0.27906976744186046</v>
-      </c>
-      <c r="D20" s="10">
-        <f>C43/C38</f>
-        <v>0.41968911917098439</v>
-      </c>
-      <c r="E20" s="10">
-        <f>D43/D38</f>
-        <v>0.66666666666666674</v>
-      </c>
-      <c r="F20" s="10">
-        <f>E43/E38</f>
-        <v>1.0820895522388061</v>
-      </c>
-      <c r="G20" s="10">
-        <f>F43/F38</f>
-        <v>1.40327868852459</v>
-      </c>
-      <c r="H20" s="10">
-        <f>G43/G38</f>
-        <v>1.8179012345679013</v>
+      <c r="C20" s="5">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+      <c r="G20" s="5">
+        <v>1</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="10">
-        <f>B48/B38</f>
-        <v>0.26744186046511625</v>
-      </c>
-      <c r="D21" s="10">
-        <f>C48/C38</f>
-        <v>0.39378238341968907</v>
-      </c>
-      <c r="E21" s="10">
-        <f>D48/D38</f>
-        <v>0.60093896713615025</v>
-      </c>
-      <c r="F21" s="10">
-        <f>E48/E38</f>
-        <v>0.9701492537313432</v>
-      </c>
-      <c r="G21" s="10">
-        <f>F48/F38</f>
-        <v>1.2426229508196722</v>
-      </c>
-      <c r="H21" s="10">
-        <f>G48/G38</f>
-        <v>1.5617283950617284</v>
+        <v>8</v>
+      </c>
+      <c r="C21" s="8">
+        <f>B43/B38</f>
+        <v>0.27906976744186046</v>
+      </c>
+      <c r="D21" s="8">
+        <f>C43/C38</f>
+        <v>0.41968911917098439</v>
+      </c>
+      <c r="E21" s="8">
+        <f>D43/D38</f>
+        <v>0.66666666666666674</v>
+      </c>
+      <c r="F21" s="8">
+        <f>E43/E38</f>
+        <v>1.0820895522388061</v>
+      </c>
+      <c r="G21" s="8">
+        <f>F43/F38</f>
+        <v>1.40327868852459</v>
+      </c>
+      <c r="H21" s="8">
+        <f>G43/G38</f>
+        <v>1.8179012345679013</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="8">
+        <f>B48/B38</f>
+        <v>0.26744186046511625</v>
+      </c>
+      <c r="D22" s="8">
+        <f>C48/C38</f>
+        <v>0.39378238341968907</v>
+      </c>
+      <c r="E22" s="8">
+        <f>D48/D38</f>
+        <v>0.60093896713615025</v>
+      </c>
+      <c r="F22" s="8">
+        <f>E48/E38</f>
+        <v>0.9701492537313432</v>
+      </c>
+      <c r="G22" s="8">
+        <f>F48/F38</f>
+        <v>1.2426229508196722</v>
+      </c>
+      <c r="H22" s="8">
+        <f>G48/G38</f>
+        <v>1.5617283950617284</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C23" s="8">
         <f>B53/B38</f>
         <v>0.73255813953488369</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D23" s="8">
         <f>C53/C38</f>
         <v>1.398963730569948</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="8">
         <f>D53/D38</f>
         <v>1.375586854460094</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F23" s="8">
         <f>E53/E38</f>
         <v>0.9253731343283581</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G23" s="8">
         <f>F53/F38</f>
         <v>0.94426229508196724</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H23" s="8">
         <f>G53/G38</f>
         <v>0.97530864197530875</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C23" s="11">
-        <f>B58/B38</f>
-        <v>0.2598954197746407</v>
-      </c>
-      <c r="D23" s="11">
-        <f t="shared" ref="D23:H23" si="5">C58/C38</f>
-        <v>0.37687839012854352</v>
-      </c>
-      <c r="E23" s="11">
-        <f t="shared" si="5"/>
-        <v>0.57476642047521598</v>
-      </c>
-      <c r="F23" s="11">
-        <f t="shared" si="5"/>
-        <v>0.71000824948220143</v>
-      </c>
-      <c r="G23" s="11">
-        <f t="shared" si="5"/>
-        <v>0.67939641020345898</v>
-      </c>
-      <c r="H23" s="11">
-        <f t="shared" si="5"/>
-        <v>0.83758036999129015</v>
-      </c>
-    </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="C24" s="2">
+        <f>B58/B38</f>
+        <v>0.63202885276682563</v>
+      </c>
+      <c r="D24" s="2">
+        <f>C58/C38</f>
+        <v>0.94005219740566826</v>
+      </c>
+      <c r="E24" s="2">
+        <f>D58/D38</f>
+        <v>1.5635544843452394</v>
+      </c>
+      <c r="F24" s="2">
+        <f>D58/E38</f>
+        <v>1.2426757655430447</v>
+      </c>
+      <c r="G24" s="2">
+        <f>E58/F38</f>
+        <v>0.80645864536337053</v>
+      </c>
+      <c r="H24" s="2">
+        <f>G58/G38</f>
+        <v>2.3319946190610743</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="2">
+        <f>B63/B38</f>
+        <v>2.067545861620331</v>
+      </c>
+      <c r="D25" s="2">
+        <f>C63/C38</f>
+        <v>3.2391680876707611</v>
+      </c>
+      <c r="E25" s="2">
+        <f>D63/D38</f>
+        <v>4.8278759500919257</v>
+      </c>
+      <c r="F25" s="2">
+        <f>E63/E38</f>
+        <v>5.7848460418539549</v>
+      </c>
+      <c r="G25" s="2">
+        <f>F63/F38</f>
+        <v>6.8705895029893114</v>
+      </c>
+      <c r="H25" s="2">
+        <f>G63/G38</f>
+        <v>6.6112347550916057</v>
+      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B34">
@@ -2089,22 +2981,22 @@
       <c r="A36" t="s">
         <v>4</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="7">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="7">
         <v>2.1700000000000001E-2</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="7">
         <v>2.8500000000000001E-2</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="7">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="7">
         <v>5.2299999999999999E-2</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="7">
         <v>6.3899999999999998E-2</v>
       </c>
     </row>
@@ -2112,22 +3004,22 @@
       <c r="A37" t="s">
         <v>5</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="7">
         <v>3.3E-3</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="7">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="7">
         <v>5.7999999999999996E-3</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="7">
         <v>0.01</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="7">
         <v>1.78E-2</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="7">
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
@@ -2135,22 +3027,22 @@
       <c r="A38" t="s">
         <v>6</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="7">
         <v>1.72E-2</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="7">
         <v>1.9300000000000001E-2</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="7">
         <v>2.1299999999999999E-2</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="7">
         <v>2.6800000000000001E-2</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="7">
         <v>3.0499999999999999E-2</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="7">
         <v>3.2399999999999998E-2</v>
       </c>
     </row>
@@ -2302,12 +3194,12 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -2336,7 +3228,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -2365,7 +3257,7 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -2388,104 +3280,589 @@
         <v>3.1600000000000003E-2</v>
       </c>
       <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K53" s="1">
+        <v>1.38371902962317E-2</v>
+      </c>
+      <c r="L53" s="1">
+        <v>1.90544023458835E-2</v>
+      </c>
+      <c r="M53">
+        <v>2.42706846029738E-2</v>
+      </c>
+      <c r="N53" s="1">
+        <v>2.81126087262468E-2</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P53" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q53" t="s">
+        <v>34</v>
+      </c>
+      <c r="R53" t="s">
+        <v>35</v>
+      </c>
+      <c r="S53" t="s">
+        <v>36</v>
+      </c>
+      <c r="T53" t="s">
+        <v>37</v>
+      </c>
+      <c r="U53" t="s">
+        <v>38</v>
+      </c>
+      <c r="V53" t="s">
+        <v>39</v>
+      </c>
+      <c r="W53" t="s">
+        <v>40</v>
+      </c>
+      <c r="X53" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="K54">
+        <v>4.1683174000870599E-2</v>
+      </c>
+      <c r="L54">
+        <v>6.3000880039182805E-2</v>
+      </c>
+      <c r="M54">
+        <v>9.7626326999087604E-2</v>
+      </c>
+      <c r="N54">
+        <v>0.11561050980246999</v>
+      </c>
+      <c r="O54" t="s">
+        <v>44</v>
+      </c>
+      <c r="P54" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>46</v>
+      </c>
+      <c r="R54" t="s">
+        <v>47</v>
+      </c>
+      <c r="S54" t="s">
+        <v>48</v>
+      </c>
+      <c r="T54" t="s">
+        <v>49</v>
+      </c>
+      <c r="U54" t="s">
+        <v>50</v>
+      </c>
+      <c r="V54" t="s">
+        <v>51</v>
+      </c>
+      <c r="W54" t="s">
+        <v>52</v>
+      </c>
+      <c r="X54" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="K55">
+        <v>3.5561788819869697E-2</v>
+      </c>
+      <c r="L55">
+        <v>6.2515944092045694E-2</v>
+      </c>
+      <c r="M55">
+        <v>8.6276205509178194E-2</v>
+      </c>
+      <c r="N55">
+        <v>0.10283375773695801</v>
+      </c>
+      <c r="O55" t="s">
+        <v>56</v>
+      </c>
+      <c r="P55" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q55" t="s">
+        <v>58</v>
+      </c>
+      <c r="R55" t="s">
+        <v>59</v>
+      </c>
+      <c r="S55" t="s">
+        <v>60</v>
+      </c>
+      <c r="T55" t="s">
+        <v>61</v>
+      </c>
+      <c r="U55" t="s">
+        <v>62</v>
+      </c>
+      <c r="V55" t="s">
+        <v>63</v>
+      </c>
+      <c r="W55" t="s">
+        <v>64</v>
+      </c>
+      <c r="X55" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>4</v>
       </c>
-      <c r="B56" s="9">
-        <v>9.34082115793833E-3</v>
-      </c>
-      <c r="C56" s="9">
-        <v>1.35053076434707E-2</v>
-      </c>
-      <c r="D56" s="9">
-        <v>1.9975851655755401E-2</v>
-      </c>
-      <c r="E56" s="9">
-        <v>2.7276046805168201E-2</v>
-      </c>
-      <c r="F56" s="9">
-        <v>3.0355218079817999E-2</v>
-      </c>
-      <c r="G56" s="9">
-        <v>3.1829496503048102E-2</v>
-      </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B56" s="7">
+        <v>1.6845549438160301E-2</v>
+      </c>
+      <c r="C56" s="7">
+        <v>2.1529046602762999E-2</v>
+      </c>
+      <c r="D56" s="7">
+        <v>3.2640080132888001E-2</v>
+      </c>
+      <c r="E56" s="7">
+        <v>4.5593027965094998E-2</v>
+      </c>
+      <c r="F56" s="7">
+        <v>5.1858849951856703E-2</v>
+      </c>
+      <c r="G56" s="7">
+        <v>5.51431246965534E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="9">
-        <v>3.1337374016955802E-3</v>
-      </c>
-      <c r="C57" s="9">
-        <v>6.39591847004222E-3</v>
-      </c>
-      <c r="D57" s="9">
-        <v>1.1512807103328601E-2</v>
-      </c>
-      <c r="E57" s="9">
-        <v>2.00197669555384E-2</v>
-      </c>
-      <c r="F57" s="9">
-        <v>2.7293249258715801E-2</v>
-      </c>
-      <c r="G57" s="9">
-        <v>3.4747742282058201E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B57" s="7">
+        <v>1.0775246030639E-2</v>
+      </c>
+      <c r="C57" s="7">
+        <v>1.8882090700266099E-2</v>
+      </c>
+      <c r="D57" s="7">
+        <v>3.0478860368313501E-2</v>
+      </c>
+      <c r="E57" s="7">
+        <v>2.3849045892305701E-2</v>
+      </c>
+      <c r="F57" s="7">
+        <v>2.71556562892072E-2</v>
+      </c>
+      <c r="G57" s="7">
+        <v>3.2551995027388897E-2</v>
+      </c>
+      <c r="K57" t="s">
+        <v>16</v>
+      </c>
+      <c r="L57" t="s">
+        <v>17</v>
+      </c>
+      <c r="M57" t="s">
+        <v>18</v>
+      </c>
+      <c r="N57" t="s">
+        <v>19</v>
+      </c>
+      <c r="O57" t="s">
+        <v>20</v>
+      </c>
+      <c r="P57" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q57" t="s">
+        <v>22</v>
+      </c>
+      <c r="R57" t="s">
+        <v>23</v>
+      </c>
+      <c r="S57" t="s">
+        <v>24</v>
+      </c>
+      <c r="T57" t="s">
+        <v>25</v>
+      </c>
+      <c r="U57" t="s">
+        <v>26</v>
+      </c>
+      <c r="V57" t="s">
+        <v>27</v>
+      </c>
+      <c r="W57" t="s">
+        <v>28</v>
+      </c>
+      <c r="X57" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="9">
-        <v>4.4702012201238202E-3</v>
-      </c>
-      <c r="C58" s="9">
-        <v>7.2737529294808903E-3</v>
-      </c>
-      <c r="D58" s="9">
-        <v>1.22425247561221E-2</v>
-      </c>
-      <c r="E58" s="9">
-        <v>1.9028221086122999E-2</v>
-      </c>
-      <c r="F58" s="9">
-        <v>2.07215905112055E-2</v>
-      </c>
-      <c r="G58" s="9">
-        <v>2.71376039877178E-2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B58" s="7">
+        <v>1.08708962675894E-2</v>
+      </c>
+      <c r="C58" s="7">
+        <v>1.8143007409929399E-2</v>
+      </c>
+      <c r="D58" s="7">
+        <v>3.3303710516553599E-2</v>
+      </c>
+      <c r="E58" s="7">
+        <v>2.4596988683582802E-2</v>
+      </c>
+      <c r="F58" s="7">
+        <v>3.5763833412296102E-2</v>
+      </c>
+      <c r="G58" s="7">
+        <v>7.5556625657578799E-2</v>
+      </c>
+      <c r="K58">
+        <v>1.1627678364187001E-2</v>
+      </c>
+      <c r="L58">
+        <v>2.03714812954175E-2</v>
+      </c>
+      <c r="M58">
+        <v>2.9259503993138501E-2</v>
+      </c>
+      <c r="N58">
+        <v>3.6944309902231798E-2</v>
+      </c>
+      <c r="O58">
+        <v>4.3279401709165603E-2</v>
+      </c>
+      <c r="P58">
+        <v>4.8766261240746199E-2</v>
+      </c>
+      <c r="Q58">
+        <v>4.9433068279657703E-2</v>
+      </c>
+      <c r="R58">
+        <v>5.4087449794570197E-2</v>
+      </c>
+      <c r="S58">
+        <v>5.8710938480798197E-2</v>
+      </c>
+      <c r="T58">
+        <v>6.2625584264784401E-2</v>
+      </c>
+      <c r="U58">
+        <v>6.6455557302738694E-2</v>
+      </c>
+      <c r="V58">
+        <v>7.0469877742787707E-2</v>
+      </c>
+      <c r="W58">
+        <v>7.4566724197574805E-2</v>
+      </c>
+      <c r="X58">
+        <v>7.8231979188317105E-2</v>
+      </c>
+      <c r="Y58">
+        <v>8.1520275850224505E-2</v>
+      </c>
+      <c r="Z58">
+        <v>8.4972826962955203E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="K59">
+        <v>1.45472965447746E-2</v>
+      </c>
+      <c r="L59">
+        <v>3.01571637670398E-2</v>
+      </c>
+      <c r="M59">
+        <v>4.3546794621815502E-2</v>
+      </c>
+      <c r="N59">
+        <v>5.6170733617979599E-2</v>
+      </c>
+      <c r="O59">
+        <v>6.6710430526945905E-2</v>
+      </c>
+      <c r="P59">
+        <v>7.7938466129045994E-2</v>
+      </c>
+      <c r="Q59">
+        <v>8.7627827091554603E-2</v>
+      </c>
+      <c r="R59">
+        <v>9.7973388536540904E-2</v>
+      </c>
+      <c r="S59">
+        <v>0.10751922242214799</v>
+      </c>
+      <c r="T59">
+        <v>0.117483879871327</v>
+      </c>
+      <c r="U59">
+        <v>0.12835410878630499</v>
+      </c>
+      <c r="V59">
+        <v>0.13916767610779401</v>
+      </c>
+      <c r="W59">
+        <v>0.15140667304164901</v>
+      </c>
+      <c r="X59">
+        <v>0.16445330411019299</v>
+      </c>
+      <c r="Y59">
+        <v>0.17588452258446599</v>
+      </c>
+      <c r="Z59">
+        <v>0.18965716862856299</v>
+      </c>
+    </row>
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B61" s="1">
+        <v>1.38371902962317E-2</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1.90544023458835E-2</v>
+      </c>
+      <c r="D61" s="1">
+        <v>2.81126087262468E-2</v>
+      </c>
+      <c r="E61" s="7">
+        <v>3.6310987258604599E-2</v>
+      </c>
+      <c r="F61" s="7">
+        <v>6.15564571812309E-2</v>
+      </c>
+      <c r="G61" s="7">
+        <v>0.113618334615791</v>
+      </c>
+      <c r="K61">
+        <v>2.2955561876052299E-2</v>
+      </c>
+      <c r="L61">
+        <v>3.6983908363027597E-2</v>
+      </c>
+      <c r="M61">
+        <v>4.77016039647618E-2</v>
+      </c>
+      <c r="N61">
+        <v>5.53456183788281E-2</v>
+      </c>
+      <c r="O61">
+        <v>6.1222616098813097E-2</v>
+      </c>
+      <c r="P61">
+        <v>6.5188825956479401E-2</v>
+      </c>
+      <c r="Q61">
+        <v>6.8005545120611299E-2</v>
+      </c>
+      <c r="R61">
+        <v>6.9997707817813795E-2</v>
+      </c>
+      <c r="S61">
+        <v>7.1022943002023206E-2</v>
+      </c>
+      <c r="T61">
+        <v>7.1779354779563501E-2</v>
+      </c>
+      <c r="U61">
+        <v>7.2282445084052099E-2</v>
+      </c>
+      <c r="V61">
+        <v>7.2202211693500107E-2</v>
+      </c>
+      <c r="W61">
+        <v>7.2212919196280603E-2</v>
+      </c>
+      <c r="X61">
+        <v>7.2064869408558094E-2</v>
+      </c>
+      <c r="Y61">
+        <v>7.1969948451658994E-2</v>
+      </c>
+      <c r="Z61">
+        <v>7.1692758685720698E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B62" s="7">
+        <v>4.1683174000870599E-2</v>
+      </c>
+      <c r="C62" s="7">
+        <v>6.3000880039182805E-2</v>
+      </c>
+      <c r="D62" s="7">
+        <v>0.11561050980246999</v>
+      </c>
+      <c r="E62" s="7">
+        <v>0.247977748976655</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0.459674222309368</v>
+      </c>
+      <c r="G62" s="7">
+        <v>0.74083044812634802</v>
+      </c>
+      <c r="K62">
+        <v>1.0775246030639E-2</v>
+      </c>
+      <c r="L62">
+        <v>1.8882090700266099E-2</v>
+      </c>
+      <c r="M62">
+        <v>2.5415255898998401E-2</v>
+      </c>
+      <c r="N62">
+        <v>3.0478860368313501E-2</v>
+      </c>
+      <c r="O62">
+        <v>3.4409804909836299E-2</v>
+      </c>
+      <c r="P62">
+        <v>3.4682600355186402E-2</v>
+      </c>
+      <c r="Q62">
+        <v>3.07346336849308E-2</v>
+      </c>
+      <c r="R62">
+        <v>2.3849045892305701E-2</v>
+      </c>
+      <c r="S62">
+        <v>2.4480568780615799E-2</v>
+      </c>
+      <c r="T62">
+        <v>2.5226886364731398E-2</v>
+      </c>
+      <c r="U62">
+        <v>2.58956211308498E-2</v>
+      </c>
+      <c r="V62">
+        <v>2.71556562892072E-2</v>
+      </c>
+      <c r="W62">
+        <v>2.83540056191008E-2</v>
+      </c>
+      <c r="X62">
+        <v>2.95252555351577E-2</v>
+      </c>
+      <c r="Y62">
+        <v>3.0504966306713299E-2</v>
+      </c>
+      <c r="Z62">
+        <v>3.2551995027388897E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>6</v>
+      </c>
+      <c r="B63" s="7">
+        <v>3.5561788819869697E-2</v>
+      </c>
+      <c r="C63" s="7">
+        <v>6.2515944092045694E-2</v>
+      </c>
+      <c r="D63" s="7">
+        <v>0.10283375773695801</v>
+      </c>
+      <c r="E63" s="7">
+        <v>0.15503387392168599</v>
+      </c>
+      <c r="F63" s="7">
+        <v>0.20955297984117399</v>
+      </c>
+      <c r="G63" s="7">
+        <v>0.21420400606496801</v>
+      </c>
+      <c r="K63">
+        <v>1.08708962675894E-2</v>
+      </c>
+      <c r="L63">
+        <v>1.8143007409929399E-2</v>
+      </c>
+      <c r="M63">
+        <v>2.54632752770028E-2</v>
+      </c>
+      <c r="N63">
+        <v>3.3303710516553599E-2</v>
+      </c>
+      <c r="O63">
+        <v>4.3018596831933702E-2</v>
+      </c>
+      <c r="P63">
+        <v>5.2379374283799303E-2</v>
+      </c>
+      <c r="Q63">
+        <v>5.16673544978829E-2</v>
+      </c>
+      <c r="R63">
+        <v>2.4596988683582802E-2</v>
+      </c>
+      <c r="S63">
+        <v>2.65079696590571E-2</v>
+      </c>
+      <c r="T63">
+        <v>2.8408653361489799E-2</v>
+      </c>
+      <c r="U63">
+        <v>3.17425827698972E-2</v>
+      </c>
+      <c r="V63">
+        <v>3.5763833412296102E-2</v>
+      </c>
+      <c r="W63">
+        <v>4.2922085866939297E-2</v>
+      </c>
+      <c r="X63">
+        <v>5.1666494594819597E-2</v>
+      </c>
+      <c r="Y63">
+        <v>6.2816313716288902E-2</v>
+      </c>
+      <c r="Z63">
+        <v>7.5556625657578799E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all state space models run
</commit_message>
<xml_diff>
--- a/Results/Forecast Evaluation Results.xlsx
+++ b/Results/Forecast Evaluation Results.xlsx
@@ -1,25 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Documents/Repositories/financial_case_studies/Results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nlralli1\Documents\Financial Case Study\financial_case_studies\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="460" windowWidth="27360" windowHeight="15820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1440" yWindow="465" windowWidth="27360" windowHeight="15825" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MAE" sheetId="1" r:id="rId1"/>
     <sheet name="RMSE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -457,7 +454,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -472,13 +469,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -504,6 +502,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -778,25 +779,25 @@
       <selection activeCell="B24" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3">
@@ -818,7 +819,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -826,180 +827,180 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <f>B35/B35</f>
+        <f t="shared" ref="C4:H4" si="0">B35/B35</f>
         <v>1</v>
       </c>
       <c r="D4">
-        <f>C35/C35</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="E4">
-        <f>D35/D35</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F4">
-        <f>E35/E35</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G4">
-        <f>F35/F35</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H4">
-        <f>G35/G35</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="2">
-        <f>B40/B35</f>
+        <f t="shared" ref="C5:H5" si="1">B40/B35</f>
         <v>1.0942028985507246</v>
       </c>
       <c r="D5" s="2">
-        <f>C40/C35</f>
+        <f t="shared" si="1"/>
         <v>1.0246913580246915</v>
       </c>
       <c r="E5" s="2">
-        <f>D40/D35</f>
+        <f t="shared" si="1"/>
         <v>0.98514851485148525</v>
       </c>
       <c r="F5" s="2">
-        <f>E40/E35</f>
+        <f t="shared" si="1"/>
         <v>0.95862068965517233</v>
       </c>
       <c r="G5" s="2">
-        <f>F40/F35</f>
+        <f t="shared" si="1"/>
         <v>0.9840000000000001</v>
       </c>
       <c r="H5" s="2">
-        <f>G40/G35</f>
+        <f t="shared" si="1"/>
         <v>1.0159453302961274</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="2">
-        <f>B45/B35</f>
+        <f t="shared" ref="C6:H6" si="2">B45/B35</f>
         <v>1.4057971014492754</v>
       </c>
       <c r="D6" s="2">
-        <f>C45/C35</f>
+        <f t="shared" si="2"/>
         <v>1.2222222222222223</v>
       </c>
       <c r="E6" s="2">
-        <f>D45/D35</f>
+        <f t="shared" si="2"/>
         <v>1.0594059405940595</v>
       </c>
       <c r="F6" s="2">
-        <f>E45/E35</f>
+        <f t="shared" si="2"/>
         <v>0.87931034482758608</v>
       </c>
       <c r="G6" s="2">
-        <f>F45/F35</f>
+        <f t="shared" si="2"/>
         <v>0.84266666666666679</v>
       </c>
       <c r="H6" s="2">
-        <f>G45/G35</f>
+        <f t="shared" si="2"/>
         <v>0.82687927107061499</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="2">
-        <f>B50/B35</f>
+        <f t="shared" ref="C7:H7" si="3">B50/B35</f>
         <v>0.63768115942028991</v>
       </c>
       <c r="D7" s="2">
-        <f>C50/C35</f>
+        <f t="shared" si="3"/>
         <v>0.69753086419753085</v>
       </c>
       <c r="E7" s="2">
-        <f>D50/D35</f>
+        <f t="shared" si="3"/>
         <v>0.76732673267326734</v>
       </c>
       <c r="F7" s="2">
-        <f>E50/E35</f>
+        <f t="shared" si="3"/>
         <v>0.52068965517241383</v>
       </c>
       <c r="G7" s="2">
-        <f>F50/F35</f>
+        <f t="shared" si="3"/>
         <v>0.38133333333333336</v>
       </c>
       <c r="H7" s="2">
-        <f>G50/G35</f>
+        <f t="shared" si="3"/>
         <v>0.33940774487471526</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C8" s="2">
-        <f>B55/B35</f>
+        <f t="shared" ref="C8:H8" si="4">B55/B35</f>
         <v>0.79192631102819566</v>
       </c>
       <c r="D8" s="2">
-        <f>C55/C35</f>
+        <f t="shared" si="4"/>
         <v>0.96816371548238278</v>
       </c>
       <c r="E8" s="2">
-        <f>D55/D35</f>
+        <f t="shared" si="4"/>
         <v>1.3578365183468268</v>
       </c>
       <c r="F8" s="2">
-        <f>E55/E35</f>
+        <f t="shared" si="4"/>
         <v>1.2623532402044171</v>
       </c>
       <c r="G8" s="2">
-        <f>F55/F35</f>
+        <f t="shared" si="4"/>
         <v>1.1703426660463014</v>
       </c>
       <c r="H8" s="2">
-        <f>G55/G35</f>
+        <f t="shared" si="4"/>
         <v>1.1452690165955284</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="2">
-        <f>B60/B35</f>
+        <f t="shared" ref="C9:H9" si="5">B60/B35</f>
         <v>0.65799731691513341</v>
       </c>
       <c r="D9" s="2">
-        <f>C60/C35</f>
+        <f t="shared" si="5"/>
         <v>0.79270483765752475</v>
       </c>
       <c r="E9" s="2">
-        <f>D60/D35</f>
+        <f t="shared" si="5"/>
         <v>0.90030676120047515</v>
       </c>
       <c r="F9" s="2">
-        <f>E60/E35</f>
+        <f t="shared" si="5"/>
         <v>0.78194680613964473</v>
       </c>
       <c r="G9" s="2">
-        <f>F60/F35</f>
+        <f t="shared" si="5"/>
         <v>0.87275749520674673</v>
       </c>
       <c r="H9" s="2">
-        <f>G60/G35</f>
+        <f t="shared" si="5"/>
         <v>1.127704110372264</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11">
@@ -1021,7 +1022,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
@@ -1029,180 +1030,180 @@
         <v>7</v>
       </c>
       <c r="C12">
-        <f>B41/B41</f>
+        <f t="shared" ref="C12:H12" si="6">B41/B41</f>
         <v>1</v>
       </c>
       <c r="D12">
-        <f>C41/C41</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="E12">
-        <f>D41/D41</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="F12">
-        <f>E41/E41</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="G12">
-        <f>F41/F41</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="H12">
-        <f>G41/G41</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="2">
-        <f>B41/B36</f>
+        <f t="shared" ref="C13:H13" si="7">B41/B36</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D13" s="2">
-        <f>C41/C36</f>
+        <f t="shared" si="7"/>
         <v>0.93103448275862077</v>
       </c>
       <c r="E13" s="2">
-        <f>D41/D36</f>
+        <f t="shared" si="7"/>
         <v>1.1142857142857141</v>
       </c>
       <c r="F13" s="2">
-        <f>E41/E36</f>
+        <f t="shared" si="7"/>
         <v>0.89583333333333337</v>
       </c>
       <c r="G13" s="2">
-        <f>F41/F36</f>
+        <f t="shared" si="7"/>
         <v>0.7</v>
       </c>
       <c r="H13" s="2">
-        <f>G41/G36</f>
+        <f t="shared" si="7"/>
         <v>0.44871794871794873</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C14" s="2">
-        <f>B46/B36</f>
+        <f t="shared" ref="C14:H14" si="8">B46/B36</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="D14" s="2">
-        <f>C46/C36</f>
+        <f t="shared" si="8"/>
         <v>0.93103448275862077</v>
       </c>
       <c r="E14" s="2">
-        <f>D46/D36</f>
+        <f t="shared" si="8"/>
         <v>1.1142857142857141</v>
       </c>
       <c r="F14" s="2">
-        <f>E46/E36</f>
+        <f t="shared" si="8"/>
         <v>0.875</v>
       </c>
       <c r="G14" s="2">
-        <f>F46/F36</f>
+        <f t="shared" si="8"/>
         <v>0.68571428571428561</v>
       </c>
       <c r="H14" s="2">
-        <f>G46/G36</f>
+        <f t="shared" si="8"/>
         <v>0.4358974358974359</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C15" s="2">
-        <f>B51/B36</f>
+        <f t="shared" ref="C15:H15" si="9">B51/B36</f>
         <v>1.8888888888888888</v>
       </c>
       <c r="D15" s="2">
-        <f>C51/C36</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="E15" s="2">
-        <f>D51/D36</f>
+        <f t="shared" si="9"/>
         <v>2.5714285714285712</v>
       </c>
       <c r="F15" s="2">
-        <f>E51/E36</f>
+        <f t="shared" si="9"/>
         <v>2.2083333333333335</v>
       </c>
       <c r="G15" s="2">
-        <f>F51/F36</f>
+        <f t="shared" si="9"/>
         <v>1.5857142857142859</v>
       </c>
       <c r="H15" s="2">
-        <f>G51/G36</f>
+        <f t="shared" si="9"/>
         <v>1.8076923076923077</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="2">
-        <f>B56/B36</f>
+        <f t="shared" ref="C16:H16" si="10">B56/B36</f>
         <v>1.9192823130175556</v>
       </c>
       <c r="D16" s="2">
-        <f>C56/C36</f>
+        <f t="shared" si="10"/>
         <v>3.1098555423629137</v>
       </c>
       <c r="E16" s="2">
-        <f>D56/D36</f>
+        <f t="shared" si="10"/>
         <v>4.0972192655231714</v>
       </c>
       <c r="F16" s="2">
-        <f>E56/E36</f>
+        <f t="shared" si="10"/>
         <v>2.6331337943585833</v>
       </c>
       <c r="G16" s="2">
-        <f>F56/F36</f>
+        <f t="shared" si="10"/>
         <v>2.0830446574182</v>
       </c>
       <c r="H16" s="2">
-        <f>G56/G36</f>
+        <f t="shared" si="10"/>
         <v>2.1171214629621411</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C17" s="2">
-        <f>B61/B36</f>
+        <f t="shared" ref="C17:H17" si="11">B61/B36</f>
         <v>8.1795421078592589</v>
       </c>
       <c r="D17" s="2">
-        <f>C61/C36</f>
+        <f t="shared" si="11"/>
         <v>12.994674452335001</v>
       </c>
       <c r="E17" s="2">
-        <f>D61/D36</f>
+        <f t="shared" si="11"/>
         <v>18.760019901231257</v>
       </c>
       <c r="F17" s="2">
-        <f>E61/E36</f>
+        <f t="shared" si="11"/>
         <v>24.172004884128544</v>
       </c>
       <c r="G17" s="2">
-        <f>F61/F36</f>
+        <f t="shared" si="11"/>
         <v>24.807203836478003</v>
       </c>
       <c r="H17" s="2">
-        <f>G61/G36</f>
+        <f t="shared" si="11"/>
         <v>25.838265197008848</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19">
@@ -1224,7 +1225,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>6</v>
       </c>
@@ -1232,179 +1233,179 @@
         <v>7</v>
       </c>
       <c r="C20">
-        <f>B47/B47</f>
+        <f t="shared" ref="C20:H20" si="12">B47/B47</f>
         <v>1</v>
       </c>
       <c r="D20">
-        <f>C47/C47</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="E20">
-        <f>D47/D47</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="F20">
-        <f>E47/E47</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="G20">
-        <f>F47/F47</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="H20">
-        <f>G47/G47</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
       <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="2">
-        <f>B42/B37</f>
+        <f t="shared" ref="C21:H21" si="13">B42/B37</f>
         <v>0.27407407407407408</v>
       </c>
       <c r="D21" s="2">
-        <f>C42/C37</f>
+        <f t="shared" si="13"/>
         <v>0.38815789473684209</v>
       </c>
       <c r="E21" s="2">
-        <f>D42/D37</f>
+        <f t="shared" si="13"/>
         <v>0.62962962962962976</v>
       </c>
       <c r="F21" s="2">
-        <f>E42/E37</f>
+        <f t="shared" si="13"/>
         <v>0.91219512195121955</v>
       </c>
       <c r="G21" s="2">
-        <f>F42/F37</f>
+        <f t="shared" si="13"/>
         <v>1.0941176470588236</v>
       </c>
       <c r="H21" s="2">
-        <f>G42/G37</f>
+        <f t="shared" si="13"/>
         <v>1.4891304347826086</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="2">
-        <f>B47/B37</f>
+        <f t="shared" ref="C22:H22" si="14">B47/B37</f>
         <v>0.25925925925925924</v>
       </c>
       <c r="D22" s="2">
-        <f>C47/C37</f>
+        <f t="shared" si="14"/>
         <v>0.36184210526315785</v>
       </c>
       <c r="E22" s="2">
-        <f>D47/D37</f>
+        <f t="shared" si="14"/>
         <v>0.54320987654320996</v>
       </c>
       <c r="F22" s="2">
-        <f>E47/E37</f>
+        <f t="shared" si="14"/>
         <v>0.76585365853658527</v>
       </c>
       <c r="G22" s="2">
-        <f>F47/F37</f>
+        <f t="shared" si="14"/>
         <v>0.90196078431372551</v>
       </c>
       <c r="H22" s="2">
-        <f>G47/G37</f>
+        <f t="shared" si="14"/>
         <v>1.1847826086956521</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C23" s="2">
-        <f>B52/B37</f>
+        <f t="shared" ref="C23:H23" si="15">B52/B37</f>
         <v>0.48148148148148145</v>
       </c>
       <c r="D23" s="2">
-        <f>C52/C37</f>
+        <f t="shared" si="15"/>
         <v>0.74342105263157887</v>
       </c>
       <c r="E23" s="2">
-        <f>D52/D37</f>
+        <f t="shared" si="15"/>
         <v>0.97530864197530875</v>
       </c>
       <c r="F23" s="2">
-        <f>E52/E37</f>
+        <f t="shared" si="15"/>
         <v>0.82439024390243887</v>
       </c>
       <c r="G23" s="2">
-        <f>F52/F37</f>
+        <f t="shared" si="15"/>
         <v>0.81176470588235294</v>
       </c>
       <c r="H23" s="2">
-        <f>G52/G37</f>
+        <f t="shared" si="15"/>
         <v>0.92028985507246375</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="2">
-        <f>B57/B37</f>
+        <f t="shared" ref="C24:H24" si="16">B57/B37</f>
         <v>0.51581563387925777</v>
       </c>
       <c r="D24" s="2">
-        <f>C57/C37</f>
+        <f t="shared" si="16"/>
         <v>0.73633405738570401</v>
       </c>
       <c r="E24" s="2">
-        <f>D57/D37</f>
+        <f t="shared" si="16"/>
         <v>1.1938080124980617</v>
       </c>
       <c r="F24" s="2">
-        <f>E57/E37</f>
+        <f t="shared" si="16"/>
         <v>0.87511521982990237</v>
       </c>
       <c r="G24" s="2">
-        <f>F57/F37</f>
+        <f t="shared" si="16"/>
         <v>0.94340042327306672</v>
       </c>
       <c r="H24" s="2">
-        <f>G57/G37</f>
+        <f t="shared" si="16"/>
         <v>1.5038884836762065</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C25" s="2">
-        <f>B62/B37</f>
+        <f t="shared" ref="C25:H25" si="17">B62/B37</f>
         <v>1.544479175027726</v>
       </c>
       <c r="D25" s="2">
-        <f>C62/C37</f>
+        <f t="shared" si="17"/>
         <v>2.4637607820055263</v>
       </c>
       <c r="E25" s="2">
-        <f>D62/D37</f>
+        <f t="shared" si="17"/>
         <v>3.9311004709065127</v>
       </c>
       <c r="F25" s="2">
-        <f>E62/E37</f>
+        <f t="shared" si="17"/>
         <v>5.0197479448860483</v>
       </c>
       <c r="G25" s="2">
-        <f>F62/F37</f>
+        <f t="shared" si="17"/>
         <v>5.6780745154984711</v>
       </c>
       <c r="H25" s="2">
-        <f>G62/G37</f>
+        <f t="shared" si="17"/>
         <v>5.2932516879768841</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1</v>
       </c>
@@ -1424,12 +1425,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>4</v>
       </c>
@@ -1452,7 +1453,7 @@
         <v>4.3900000000000002E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>7.7999999999999996E-3</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
@@ -1498,12 +1499,12 @@
         <v>2.76E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>4</v>
       </c>
@@ -1526,7 +1527,7 @@
         <v>4.4600000000000001E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>5</v>
       </c>
@@ -1549,7 +1550,7 @@
         <v>3.5000000000000001E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
@@ -1572,12 +1573,12 @@
         <v>4.1099999999999998E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>4</v>
       </c>
@@ -1600,7 +1601,7 @@
         <v>3.6299999999999999E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>5</v>
       </c>
@@ -1623,7 +1624,7 @@
         <v>3.3999999999999998E-3</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>6</v>
       </c>
@@ -1646,12 +1647,12 @@
         <v>3.27E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>4</v>
       </c>
@@ -1681,7 +1682,7 @@
       <c r="O50" s="1"/>
       <c r="P50" s="1"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>5</v>
       </c>
@@ -1711,7 +1712,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>6</v>
       </c>
@@ -1741,12 +1742,12 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -1817,7 +1818,7 @@
         <v>1.6336539195234499E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>5</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>4.2497415078740899E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>6</v>
       </c>
@@ -1959,12 +1960,12 @@
         <v>6.9800686445864096E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>4</v>
       </c>
@@ -2035,7 +2036,7 @@
         <v>5.0277309828543698E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -2106,7 +2107,7 @@
         <v>1.6513547411104699E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>6</v>
       </c>
@@ -2177,7 +2178,7 @@
         <v>4.1507322149463302E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K64" t="s">
         <v>69</v>
       </c>
@@ -2227,7 +2228,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K65" t="s">
         <v>85</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="11:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="11:26" x14ac:dyDescent="0.25">
       <c r="K66" t="s">
         <v>101</v>
       </c>
@@ -2341,12 +2342,12 @@
   <dimension ref="A1:Z63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
@@ -2362,7 +2363,7 @@
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5">
@@ -2384,7 +2385,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -2410,156 +2411,156 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8">
-        <f>B41/B36</f>
+      <c r="C5" s="10">
+        <f t="shared" ref="C5:H5" si="0">B41/B36</f>
         <v>1.3666666666666667</v>
       </c>
-      <c r="D5" s="8">
-        <f>C41/C36</f>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
         <v>1.1612903225806452</v>
       </c>
-      <c r="E5" s="8">
-        <f>D41/D36</f>
+      <c r="E5" s="10">
+        <f t="shared" si="0"/>
         <v>0.96491228070175439</v>
       </c>
-      <c r="F5" s="8">
-        <f>E41/E36</f>
+      <c r="F5" s="10">
+        <f t="shared" si="0"/>
         <v>0.83170731707317069</v>
       </c>
-      <c r="G5" s="8">
-        <f>F41/F36</f>
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
         <v>0.79923518164435947</v>
       </c>
-      <c r="H5" s="8">
-        <f>G41/G36</f>
+      <c r="H5" s="10">
+        <f t="shared" si="0"/>
         <v>0.77151799687010947</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8">
-        <f>B46/B36</f>
+      <c r="C6" s="10">
+        <f t="shared" ref="C6:H6" si="1">B46/B36</f>
         <v>1.3666666666666667</v>
       </c>
-      <c r="D6" s="8">
-        <f>C46/C36</f>
+      <c r="D6" s="10">
+        <f t="shared" si="1"/>
         <v>1.1520737327188941</v>
       </c>
-      <c r="E6" s="8">
-        <f>D46/D36</f>
+      <c r="E6" s="10">
+        <f t="shared" si="1"/>
         <v>0.94736842105263153</v>
       </c>
-      <c r="F6" s="8">
-        <f>E46/E36</f>
+      <c r="F6" s="10">
+        <f t="shared" si="1"/>
         <v>0.80487804878048785</v>
       </c>
-      <c r="G6" s="8">
-        <f>F46/F36</f>
+      <c r="G6" s="10">
+        <f t="shared" si="1"/>
         <v>0.76099426386233271</v>
       </c>
-      <c r="H6" s="8">
-        <f>G46/G36</f>
+      <c r="H6" s="10">
+        <f t="shared" si="1"/>
         <v>0.72300469483568075</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="8">
-        <f>B51/B36</f>
+      <c r="C7" s="10">
+        <f t="shared" ref="C7:H7" si="2">B51/B36</f>
         <v>0.78333333333333333</v>
       </c>
-      <c r="D7" s="8">
-        <f>C51/C36</f>
+      <c r="D7" s="10">
+        <f t="shared" si="2"/>
         <v>0.87096774193548387</v>
       </c>
-      <c r="E7" s="8">
-        <f>D51/D36</f>
+      <c r="E7" s="10">
+        <f t="shared" si="2"/>
         <v>0.94035087719298249</v>
       </c>
-      <c r="F7" s="8">
-        <f>E51/E36</f>
+      <c r="F7" s="10">
+        <f t="shared" si="2"/>
         <v>0.51707317073170733</v>
       </c>
-      <c r="G7" s="8">
-        <f>F51/F36</f>
+      <c r="G7" s="10">
+        <f t="shared" si="2"/>
         <v>0.39388145315487572</v>
       </c>
-      <c r="H7" s="8">
-        <f>G51/G36</f>
+      <c r="H7" s="10">
+        <f t="shared" si="2"/>
         <v>0.31611893583724571</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="10">
         <f>B56/B36</f>
         <v>0.93586385767557234</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="10">
         <f>C56/C36</f>
         <v>0.99212196326096769</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="10">
         <f>D56/D36</f>
         <v>1.1452659695750176</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="10">
         <f>D56/E36</f>
         <v>0.79609951543629265</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="10">
         <f>E56/F36</f>
         <v>0.87175961692342252</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="10">
         <f>G56/G36</f>
         <v>0.86295969791163385</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C9" s="2">
-        <f>B61/B36</f>
+      <c r="C9" s="11">
+        <f t="shared" ref="C9:H9" si="3">B61/B36</f>
         <v>0.76873279423509444</v>
       </c>
-      <c r="D9" s="2">
-        <f>C61/C36</f>
+      <c r="D9" s="11">
+        <f t="shared" si="3"/>
         <v>0.87808305741398618</v>
       </c>
-      <c r="E9" s="2">
-        <f>D61/D36</f>
+      <c r="E9" s="11">
+        <f t="shared" si="3"/>
         <v>0.98640732372795781</v>
       </c>
-      <c r="F9" s="2">
-        <f>E61/E36</f>
+      <c r="F9" s="11">
+        <f t="shared" si="3"/>
         <v>0.88563383557572184</v>
       </c>
-      <c r="G9" s="2">
-        <f>F61/F36</f>
+      <c r="G9" s="11">
+        <f t="shared" si="3"/>
         <v>1.176987709010151</v>
       </c>
-      <c r="H9" s="2">
-        <f>G61/G36</f>
+      <c r="H9" s="11">
+        <f t="shared" si="3"/>
         <v>1.7780647044724727</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5">
@@ -2581,7 +2582,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -2607,156 +2608,156 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="8">
-        <f>B42/B37</f>
+      <c r="C13" s="10">
+        <f t="shared" ref="C13:H13" si="4">B42/B37</f>
         <v>0.72727272727272718</v>
       </c>
-      <c r="D13" s="8">
-        <f>C42/C37</f>
+      <c r="D13" s="10">
+        <f t="shared" si="4"/>
         <v>1.027027027027027</v>
       </c>
-      <c r="E13" s="8">
-        <f>D42/D37</f>
+      <c r="E13" s="10">
+        <f t="shared" si="4"/>
         <v>0.94827586206896552</v>
       </c>
-      <c r="F13" s="8">
-        <f>E42/E37</f>
+      <c r="F13" s="10">
+        <f t="shared" si="4"/>
         <v>0.54</v>
       </c>
-      <c r="G13" s="8">
-        <f>F42/F37</f>
+      <c r="G13" s="10">
+        <f t="shared" si="4"/>
         <v>0.3202247191011236</v>
       </c>
-      <c r="H13" s="8">
-        <f>G42/G37</f>
+      <c r="H13" s="10">
+        <f t="shared" si="4"/>
         <v>0.17355371900826447</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="8">
-        <f>B47/B37</f>
+      <c r="C14" s="10">
+        <f t="shared" ref="C14:H14" si="5">B47/B37</f>
         <v>0.69696969696969702</v>
       </c>
-      <c r="D14" s="8">
-        <f>C47/C37</f>
+      <c r="D14" s="10">
+        <f t="shared" si="5"/>
         <v>0.97297297297297292</v>
       </c>
-      <c r="E14" s="8">
-        <f>D47/D37</f>
+      <c r="E14" s="10">
+        <f t="shared" si="5"/>
         <v>0.86206896551724144</v>
       </c>
-      <c r="F14" s="8">
-        <f>E47/E37</f>
+      <c r="F14" s="10">
+        <f t="shared" si="5"/>
         <v>0.52</v>
       </c>
-      <c r="G14" s="8">
-        <f>F47/F37</f>
+      <c r="G14" s="10">
+        <f t="shared" si="5"/>
         <v>0.33146067415730335</v>
       </c>
-      <c r="H14" s="8">
-        <f>G47/G37</f>
+      <c r="H14" s="10">
+        <f t="shared" si="5"/>
         <v>0.17355371900826447</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C15" s="8">
-        <f>B52/B37</f>
+      <c r="C15" s="10">
+        <f t="shared" ref="C15:H15" si="6">B52/B37</f>
         <v>4.5757575757575761</v>
       </c>
-      <c r="D15" s="8">
-        <f>C52/C37</f>
+      <c r="D15" s="10">
+        <f t="shared" si="6"/>
         <v>6.6216216216216219</v>
       </c>
-      <c r="E15" s="8">
-        <f>D52/D37</f>
+      <c r="E15" s="10">
+        <f t="shared" si="6"/>
         <v>3.0689655172413794</v>
       </c>
-      <c r="F15" s="8">
-        <f>E52/E37</f>
+      <c r="F15" s="10">
+        <f t="shared" si="6"/>
         <v>1.68</v>
       </c>
-      <c r="G15" s="8">
-        <f>F52/F37</f>
+      <c r="G15" s="10">
+        <f t="shared" si="6"/>
         <v>0.9044943820224719</v>
       </c>
-      <c r="H15" s="8">
-        <f>G52/G37</f>
+      <c r="H15" s="10">
+        <f t="shared" si="6"/>
         <v>0.79752066115702491</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="10">
         <f>B57/B37</f>
         <v>3.2652260698906064</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="10">
         <f>C57/C37</f>
         <v>5.1032677568286751</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="10">
         <f>D57/D37</f>
         <v>5.2549759255712933</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="10">
         <f>D57/E37</f>
         <v>3.0478860368313501</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="10">
         <f>E57/F37</f>
         <v>1.3398340388935788</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="10">
         <f>G57/G37</f>
         <v>1.3451237614623512</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="2">
-        <f>B62/B37</f>
+      <c r="C17" s="11">
+        <f t="shared" ref="C17:H17" si="7">B62/B37</f>
         <v>12.631264848748666</v>
       </c>
-      <c r="D17" s="2">
-        <f>C62/C37</f>
+      <c r="D17" s="11">
+        <f t="shared" si="7"/>
         <v>17.027264875454811</v>
       </c>
-      <c r="E17" s="2">
-        <f>D62/D37</f>
+      <c r="E17" s="11">
+        <f t="shared" si="7"/>
         <v>19.93284651766724</v>
       </c>
-      <c r="F17" s="2">
-        <f>E62/E37</f>
+      <c r="F17" s="11">
+        <f t="shared" si="7"/>
         <v>24.797774897665501</v>
       </c>
-      <c r="G17" s="2">
-        <f>F62/F37</f>
+      <c r="G17" s="11">
+        <f t="shared" si="7"/>
         <v>25.824394511762247</v>
       </c>
-      <c r="H17" s="2">
-        <f>G62/G37</f>
+      <c r="H17" s="11">
+        <f t="shared" si="7"/>
         <v>30.612828434973061</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5">
@@ -2778,7 +2779,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
@@ -2804,155 +2805,155 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="8">
-        <f>B43/B38</f>
+      <c r="C21" s="10">
+        <f t="shared" ref="C21:H21" si="8">B43/B38</f>
         <v>0.27906976744186046</v>
       </c>
-      <c r="D21" s="8">
-        <f>C43/C38</f>
+      <c r="D21" s="10">
+        <f t="shared" si="8"/>
         <v>0.41968911917098439</v>
       </c>
-      <c r="E21" s="8">
-        <f>D43/D38</f>
+      <c r="E21" s="10">
+        <f t="shared" si="8"/>
         <v>0.66666666666666674</v>
       </c>
-      <c r="F21" s="8">
-        <f>E43/E38</f>
+      <c r="F21" s="10">
+        <f t="shared" si="8"/>
         <v>1.0820895522388061</v>
       </c>
-      <c r="G21" s="8">
-        <f>F43/F38</f>
+      <c r="G21" s="10">
+        <f t="shared" si="8"/>
         <v>1.40327868852459</v>
       </c>
-      <c r="H21" s="8">
-        <f>G43/G38</f>
+      <c r="H21" s="10">
+        <f t="shared" si="8"/>
         <v>1.8179012345679013</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="8">
-        <f>B48/B38</f>
+      <c r="C22" s="10">
+        <f t="shared" ref="C22:H22" si="9">B48/B38</f>
         <v>0.26744186046511625</v>
       </c>
-      <c r="D22" s="8">
-        <f>C48/C38</f>
+      <c r="D22" s="10">
+        <f t="shared" si="9"/>
         <v>0.39378238341968907</v>
       </c>
-      <c r="E22" s="8">
-        <f>D48/D38</f>
+      <c r="E22" s="10">
+        <f t="shared" si="9"/>
         <v>0.60093896713615025</v>
       </c>
-      <c r="F22" s="8">
-        <f>E48/E38</f>
+      <c r="F22" s="10">
+        <f t="shared" si="9"/>
         <v>0.9701492537313432</v>
       </c>
-      <c r="G22" s="8">
-        <f>F48/F38</f>
+      <c r="G22" s="10">
+        <f t="shared" si="9"/>
         <v>1.2426229508196722</v>
       </c>
-      <c r="H22" s="8">
-        <f>G48/G38</f>
+      <c r="H22" s="10">
+        <f t="shared" si="9"/>
         <v>1.5617283950617284</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="8">
-        <f>B53/B38</f>
+      <c r="C23" s="10">
+        <f t="shared" ref="C23:H23" si="10">B53/B38</f>
         <v>0.73255813953488369</v>
       </c>
-      <c r="D23" s="8">
-        <f>C53/C38</f>
+      <c r="D23" s="10">
+        <f t="shared" si="10"/>
         <v>1.398963730569948</v>
       </c>
-      <c r="E23" s="8">
-        <f>D53/D38</f>
+      <c r="E23" s="10">
+        <f t="shared" si="10"/>
         <v>1.375586854460094</v>
       </c>
-      <c r="F23" s="8">
-        <f>E53/E38</f>
+      <c r="F23" s="10">
+        <f t="shared" si="10"/>
         <v>0.9253731343283581</v>
       </c>
-      <c r="G23" s="8">
-        <f>F53/F38</f>
+      <c r="G23" s="10">
+        <f t="shared" si="10"/>
         <v>0.94426229508196724</v>
       </c>
-      <c r="H23" s="8">
-        <f>G53/G38</f>
+      <c r="H23" s="10">
+        <f t="shared" si="10"/>
         <v>0.97530864197530875</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="11">
         <f>B58/B38</f>
         <v>0.63202885276682563</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="11">
         <f>C58/C38</f>
         <v>0.94005219740566826</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="11">
         <f>D58/D38</f>
         <v>1.5635544843452394</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="11">
         <f>D58/E38</f>
         <v>1.2426757655430447</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="11">
         <f>E58/F38</f>
         <v>0.80645864536337053</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="11">
         <f>G58/G38</f>
         <v>2.3319946190610743</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="2">
-        <f>B63/B38</f>
+      <c r="C25" s="11">
+        <f t="shared" ref="C25:H25" si="11">B63/B38</f>
         <v>2.067545861620331</v>
       </c>
-      <c r="D25" s="2">
-        <f>C63/C38</f>
+      <c r="D25" s="11">
+        <f t="shared" si="11"/>
         <v>3.2391680876707611</v>
       </c>
-      <c r="E25" s="2">
-        <f>D63/D38</f>
+      <c r="E25" s="11">
+        <f t="shared" si="11"/>
         <v>4.8278759500919257</v>
       </c>
-      <c r="F25" s="2">
-        <f>E63/E38</f>
+      <c r="F25" s="11">
+        <f t="shared" si="11"/>
         <v>5.7848460418539549</v>
       </c>
-      <c r="G25" s="2">
-        <f>F63/F38</f>
+      <c r="G25" s="11">
+        <f t="shared" si="11"/>
         <v>6.8705895029893114</v>
       </c>
-      <c r="H25" s="2">
-        <f>G63/G38</f>
+      <c r="H25" s="11">
+        <f t="shared" si="11"/>
         <v>6.6112347550916057</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>1</v>
       </c>
@@ -2972,12 +2973,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -3000,7 +3001,7 @@
         <v>6.3899999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>5</v>
       </c>
@@ -3023,7 +3024,7 @@
         <v>2.4199999999999999E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -3046,12 +3047,12 @@
         <v>3.2399999999999998E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>4</v>
       </c>
@@ -3074,7 +3075,7 @@
         <v>4.9299999999999997E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>5</v>
       </c>
@@ -3097,7 +3098,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>6</v>
       </c>
@@ -3120,12 +3121,12 @@
         <v>5.8900000000000001E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>4</v>
       </c>
@@ -3148,7 +3149,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>4.1999999999999997E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>6</v>
       </c>
@@ -3194,12 +3195,12 @@
         <v>5.0599999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
@@ -3228,7 +3229,7 @@
       <c r="O51" s="1"/>
       <c r="P51" s="1"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -3257,7 +3258,7 @@
       <c r="O52" s="1"/>
       <c r="P52" s="1"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>6</v>
       </c>
@@ -3329,7 +3330,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K54">
         <v>4.1683174000870599E-2</v>
       </c>
@@ -3379,7 +3380,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -3432,7 +3433,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>4</v>
       </c>
@@ -3455,7 +3456,7 @@
         <v>5.51431246965534E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -3526,7 +3527,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -3597,7 +3598,7 @@
         <v>8.4972826962955203E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="K59">
         <v>1.45472965447746E-2</v>
       </c>
@@ -3647,12 +3648,12 @@
         <v>0.18965716862856299</v>
       </c>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>4</v>
       </c>
@@ -3723,7 +3724,7 @@
         <v>7.1692758685720698E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>3.2551995027388897E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>6</v>
       </c>

</xml_diff>